<commit_message>
I feel the need.. the need for speed.
</commit_message>
<xml_diff>
--- a/BW Specific Fault Layout Toyopuc V9.xlsx
+++ b/BW Specific Fault Layout Toyopuc V9.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mydocs.toyota.com/personal/jonathan_shambaugh_toyota_com/Documents/Documents/Other/Code/EDC Deployment/EDC-Deployment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\459630\OneDrive - TMNA\Documents\Other\Code\EDC Deployment\EDC-Deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_97C101C617C95CB9D835EE17340732D18FECCBB9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{490C5F80-839E-4AD5-A840-AA14A5A3B4AB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327BD052-B307-4990-98F0-BACA79D3F163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5039" uniqueCount="4080">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4892" uniqueCount="4080">
   <si>
     <t>EDC BIT LAYOUT</t>
   </si>
@@ -12960,14 +12960,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -12978,8 +12978,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -13326,8 +13326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2050"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A1817" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G1731" sqref="G1731"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13342,8 +13342,8 @@
     <col min="9" max="9" width="19.44140625" style="5" customWidth="1"/>
     <col min="10" max="12" width="8.88671875" style="5" customWidth="1"/>
     <col min="13" max="13" width="18" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="8.88671875" style="5" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="5"/>
+    <col min="14" max="18" width="8.88671875" style="5" customWidth="1"/>
+    <col min="19" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -50215,9 +50215,7 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1827" s="5" t="s">
-        <v>3627</v>
-      </c>
+      <c r="F1827"/>
       <c r="G1827" s="49"/>
     </row>
     <row r="1828" spans="1:7" x14ac:dyDescent="0.3">
@@ -50238,9 +50236,7 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1828" s="5" t="s">
-        <v>3629</v>
-      </c>
+      <c r="F1828"/>
       <c r="G1828" s="49"/>
     </row>
     <row r="1829" spans="1:7" x14ac:dyDescent="0.3">
@@ -50261,9 +50257,7 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1829" s="5" t="s">
-        <v>3631</v>
-      </c>
+      <c r="F1829"/>
       <c r="G1829" s="49"/>
     </row>
     <row r="1830" spans="1:7" x14ac:dyDescent="0.3">
@@ -50284,9 +50278,7 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1830" s="5" t="s">
-        <v>3633</v>
-      </c>
+      <c r="F1830"/>
       <c r="G1830" s="49"/>
     </row>
     <row r="1831" spans="1:7" x14ac:dyDescent="0.3">
@@ -50307,9 +50299,7 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1831" s="5" t="s">
-        <v>3635</v>
-      </c>
+      <c r="F1831"/>
       <c r="G1831" s="49"/>
     </row>
     <row r="1832" spans="1:7" x14ac:dyDescent="0.3">
@@ -50330,9 +50320,7 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1832" s="5" t="s">
-        <v>3637</v>
-      </c>
+      <c r="F1832"/>
       <c r="G1832" s="49"/>
     </row>
     <row r="1833" spans="1:7" x14ac:dyDescent="0.3">
@@ -50353,9 +50341,7 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1833" s="5" t="s">
-        <v>3639</v>
-      </c>
+      <c r="F1833"/>
       <c r="G1833" s="49"/>
     </row>
     <row r="1834" spans="1:7" x14ac:dyDescent="0.3">
@@ -50376,9 +50362,7 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1834" s="5" t="s">
-        <v>3641</v>
-      </c>
+      <c r="F1834"/>
       <c r="G1834" s="49"/>
     </row>
     <row r="1835" spans="1:7" x14ac:dyDescent="0.3">
@@ -50399,9 +50383,7 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1835" s="5" t="s">
-        <v>3643</v>
-      </c>
+      <c r="F1835"/>
       <c r="G1835" s="49"/>
     </row>
     <row r="1836" spans="1:7" x14ac:dyDescent="0.3">
@@ -50422,9 +50404,6 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1836" s="5" t="s">
-        <v>3645</v>
-      </c>
       <c r="G1836" s="49"/>
     </row>
     <row r="1837" spans="1:7" x14ac:dyDescent="0.3">
@@ -50445,9 +50424,6 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1837" s="5" t="s">
-        <v>3647</v>
-      </c>
       <c r="G1837" s="49"/>
     </row>
     <row r="1838" spans="1:7" x14ac:dyDescent="0.3">
@@ -50468,9 +50444,7 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1838" s="5" t="s">
-        <v>3649</v>
-      </c>
+      <c r="F1838"/>
       <c r="G1838" s="49"/>
     </row>
     <row r="1839" spans="1:7" x14ac:dyDescent="0.3">
@@ -50491,9 +50465,7 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1839" s="5" t="s">
-        <v>3651</v>
-      </c>
+      <c r="F1839"/>
       <c r="G1839" s="49"/>
     </row>
     <row r="1840" spans="1:7" x14ac:dyDescent="0.3">
@@ -50514,9 +50486,7 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1840" s="5" t="s">
-        <v>3653</v>
-      </c>
+      <c r="F1840"/>
       <c r="G1840" s="49"/>
     </row>
     <row r="1841" spans="1:7" x14ac:dyDescent="0.3">
@@ -50537,9 +50507,7 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1841" s="5" t="s">
-        <v>3655</v>
-      </c>
+      <c r="F1841"/>
       <c r="G1841" s="49"/>
     </row>
     <row r="1842" spans="1:7" x14ac:dyDescent="0.3">
@@ -50560,9 +50528,7 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1842" s="5" t="s">
-        <v>3657</v>
-      </c>
+      <c r="F1842"/>
       <c r="G1842" s="49"/>
     </row>
     <row r="1843" spans="1:7" x14ac:dyDescent="0.3">
@@ -50583,9 +50549,7 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1843" s="5" t="s">
-        <v>3659</v>
-      </c>
+      <c r="F1843"/>
       <c r="G1843" s="49"/>
     </row>
     <row r="1844" spans="1:7" x14ac:dyDescent="0.3">
@@ -50606,9 +50570,7 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1844" s="5" t="s">
-        <v>3661</v>
-      </c>
+      <c r="F1844"/>
       <c r="G1844" s="49"/>
     </row>
     <row r="1845" spans="1:7" x14ac:dyDescent="0.3">
@@ -50629,9 +50591,7 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1845" s="5" t="s">
-        <v>3663</v>
-      </c>
+      <c r="F1845"/>
       <c r="G1845" s="49"/>
     </row>
     <row r="1846" spans="1:7" x14ac:dyDescent="0.3">
@@ -50652,9 +50612,7 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1846" s="5" t="s">
-        <v>3665</v>
-      </c>
+      <c r="F1846"/>
       <c r="G1846" s="49"/>
     </row>
     <row r="1847" spans="1:7" x14ac:dyDescent="0.3">
@@ -50675,9 +50633,7 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1847" s="5" t="s">
-        <v>3667</v>
-      </c>
+      <c r="F1847"/>
       <c r="G1847" s="49"/>
     </row>
     <row r="1848" spans="1:7" x14ac:dyDescent="0.3">
@@ -50698,9 +50654,7 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1848" s="5" t="s">
-        <v>3669</v>
-      </c>
+      <c r="F1848"/>
       <c r="G1848" s="49"/>
     </row>
     <row r="1849" spans="1:7" x14ac:dyDescent="0.3">
@@ -50721,9 +50675,7 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1849" s="5" t="s">
-        <v>3671</v>
-      </c>
+      <c r="F1849"/>
       <c r="G1849" s="49"/>
     </row>
     <row r="1850" spans="1:7" x14ac:dyDescent="0.3">
@@ -50744,9 +50696,7 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1850" s="5" t="s">
-        <v>3673</v>
-      </c>
+      <c r="F1850"/>
       <c r="G1850" s="49"/>
     </row>
     <row r="1851" spans="1:7" x14ac:dyDescent="0.3">
@@ -50767,9 +50717,6 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1851" s="5" t="s">
-        <v>3675</v>
-      </c>
       <c r="G1851" s="49"/>
     </row>
     <row r="1852" spans="1:7" x14ac:dyDescent="0.3">
@@ -50790,9 +50737,6 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1852" s="5" t="s">
-        <v>3677</v>
-      </c>
       <c r="G1852" s="49"/>
     </row>
     <row r="1853" spans="1:7" x14ac:dyDescent="0.3">
@@ -50813,9 +50757,6 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1853" s="5" t="s">
-        <v>3679</v>
-      </c>
       <c r="G1853" s="49"/>
     </row>
     <row r="1854" spans="1:7" x14ac:dyDescent="0.3">
@@ -50836,9 +50777,6 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1854" s="5" t="s">
-        <v>3681</v>
-      </c>
       <c r="G1854" s="49"/>
     </row>
     <row r="1855" spans="1:7" x14ac:dyDescent="0.3">
@@ -50859,9 +50797,6 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1855" s="5" t="s">
-        <v>3683</v>
-      </c>
       <c r="G1855" s="49"/>
     </row>
     <row r="1856" spans="1:7" x14ac:dyDescent="0.3">
@@ -50882,9 +50817,6 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1856" s="5" t="s">
-        <v>3685</v>
-      </c>
       <c r="G1856" s="49"/>
     </row>
     <row r="1857" spans="1:7" x14ac:dyDescent="0.3">
@@ -50905,9 +50837,6 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1857" s="5" t="s">
-        <v>3687</v>
-      </c>
       <c r="G1857" s="49"/>
     </row>
     <row r="1858" spans="1:7" x14ac:dyDescent="0.3">
@@ -50928,9 +50857,6 @@
         <f t="shared" si="57"/>
         <v>12</v>
       </c>
-      <c r="F1858" s="5" t="s">
-        <v>3689</v>
-      </c>
       <c r="G1858" s="49"/>
     </row>
     <row r="1859" spans="1:7" x14ac:dyDescent="0.3">
@@ -50951,9 +50877,7 @@
         <f t="shared" ref="E1859:E1922" si="59">LEN(D1859)</f>
         <v>12</v>
       </c>
-      <c r="F1859" s="5" t="s">
-        <v>3691</v>
-      </c>
+      <c r="F1859"/>
       <c r="G1859" s="49"/>
     </row>
     <row r="1860" spans="1:7" x14ac:dyDescent="0.3">
@@ -50974,9 +50898,7 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1860" s="5" t="s">
-        <v>3693</v>
-      </c>
+      <c r="F1860"/>
       <c r="G1860" s="49"/>
     </row>
     <row r="1861" spans="1:7" x14ac:dyDescent="0.3">
@@ -50997,9 +50919,7 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1861" s="5" t="s">
-        <v>3695</v>
-      </c>
+      <c r="F1861"/>
       <c r="G1861" s="49"/>
     </row>
     <row r="1862" spans="1:7" x14ac:dyDescent="0.3">
@@ -51020,9 +50940,7 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1862" s="5" t="s">
-        <v>3697</v>
-      </c>
+      <c r="F1862"/>
       <c r="G1862" s="49"/>
     </row>
     <row r="1863" spans="1:7" x14ac:dyDescent="0.3">
@@ -51043,9 +50961,7 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1863" s="5" t="s">
-        <v>3699</v>
-      </c>
+      <c r="F1863"/>
       <c r="G1863" s="49"/>
     </row>
     <row r="1864" spans="1:7" x14ac:dyDescent="0.3">
@@ -51066,9 +50982,7 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1864" s="5" t="s">
-        <v>3701</v>
-      </c>
+      <c r="F1864"/>
       <c r="G1864" s="49"/>
     </row>
     <row r="1865" spans="1:7" x14ac:dyDescent="0.3">
@@ -51089,9 +51003,7 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1865" s="5" t="s">
-        <v>3703</v>
-      </c>
+      <c r="F1865"/>
       <c r="G1865" s="49"/>
     </row>
     <row r="1866" spans="1:7" x14ac:dyDescent="0.3">
@@ -51112,9 +51024,7 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1866" s="5" t="s">
-        <v>3705</v>
-      </c>
+      <c r="F1866"/>
       <c r="G1866" s="49"/>
     </row>
     <row r="1867" spans="1:7" x14ac:dyDescent="0.3">
@@ -51135,9 +51045,7 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1867" s="5" t="s">
-        <v>3707</v>
-      </c>
+      <c r="F1867"/>
       <c r="G1867" s="49"/>
     </row>
     <row r="1868" spans="1:7" x14ac:dyDescent="0.3">
@@ -51158,9 +51066,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1868" s="5" t="s">
-        <v>3709</v>
-      </c>
       <c r="G1868" s="49"/>
     </row>
     <row r="1869" spans="1:7" x14ac:dyDescent="0.3">
@@ -51181,9 +51086,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1869" s="5" t="s">
-        <v>3711</v>
-      </c>
       <c r="G1869" s="49"/>
     </row>
     <row r="1870" spans="1:7" x14ac:dyDescent="0.3">
@@ -51204,9 +51106,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1870" s="5" t="s">
-        <v>3713</v>
-      </c>
       <c r="G1870" s="49"/>
     </row>
     <row r="1871" spans="1:7" x14ac:dyDescent="0.3">
@@ -51227,9 +51126,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1871" s="5" t="s">
-        <v>3715</v>
-      </c>
       <c r="G1871" s="49"/>
     </row>
     <row r="1872" spans="1:7" x14ac:dyDescent="0.3">
@@ -51250,9 +51146,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1872" s="5" t="s">
-        <v>3717</v>
-      </c>
       <c r="G1872" s="49"/>
     </row>
     <row r="1873" spans="1:7" x14ac:dyDescent="0.3">
@@ -51273,9 +51166,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1873" s="5" t="s">
-        <v>3719</v>
-      </c>
       <c r="G1873" s="49"/>
     </row>
     <row r="1874" spans="1:7" x14ac:dyDescent="0.3">
@@ -51296,9 +51186,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1874" s="5" t="s">
-        <v>3721</v>
-      </c>
       <c r="G1874" s="49"/>
     </row>
     <row r="1875" spans="1:7" x14ac:dyDescent="0.3">
@@ -51319,9 +51206,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1875" s="5" t="s">
-        <v>3723</v>
-      </c>
       <c r="G1875" s="49"/>
     </row>
     <row r="1876" spans="1:7" x14ac:dyDescent="0.3">
@@ -51342,9 +51226,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1876" s="5" t="s">
-        <v>3725</v>
-      </c>
       <c r="G1876" s="49"/>
     </row>
     <row r="1877" spans="1:7" x14ac:dyDescent="0.3">
@@ -51365,9 +51246,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1877" s="5" t="s">
-        <v>3727</v>
-      </c>
       <c r="G1877" s="49"/>
     </row>
     <row r="1878" spans="1:7" x14ac:dyDescent="0.3">
@@ -51388,9 +51266,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1878" s="5" t="s">
-        <v>3729</v>
-      </c>
       <c r="G1878" s="49"/>
     </row>
     <row r="1879" spans="1:7" x14ac:dyDescent="0.3">
@@ -51411,9 +51286,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1879" s="5" t="s">
-        <v>3731</v>
-      </c>
       <c r="G1879" s="49"/>
     </row>
     <row r="1880" spans="1:7" x14ac:dyDescent="0.3">
@@ -51434,9 +51306,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1880" s="5" t="s">
-        <v>3733</v>
-      </c>
       <c r="G1880" s="49"/>
     </row>
     <row r="1881" spans="1:7" x14ac:dyDescent="0.3">
@@ -51457,9 +51326,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1881" s="5" t="s">
-        <v>3735</v>
-      </c>
       <c r="G1881" s="49"/>
     </row>
     <row r="1882" spans="1:7" x14ac:dyDescent="0.3">
@@ -51480,9 +51346,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1882" s="5" t="s">
-        <v>3737</v>
-      </c>
       <c r="G1882" s="49"/>
     </row>
     <row r="1883" spans="1:7" x14ac:dyDescent="0.3">
@@ -51503,9 +51366,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1883" s="5" t="s">
-        <v>3739</v>
-      </c>
       <c r="G1883" s="49"/>
     </row>
     <row r="1884" spans="1:7" x14ac:dyDescent="0.3">
@@ -51526,9 +51386,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1884" s="5" t="s">
-        <v>3741</v>
-      </c>
       <c r="G1884" s="49"/>
     </row>
     <row r="1885" spans="1:7" x14ac:dyDescent="0.3">
@@ -51549,9 +51406,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1885" s="5" t="s">
-        <v>3743</v>
-      </c>
       <c r="G1885" s="49"/>
     </row>
     <row r="1886" spans="1:7" x14ac:dyDescent="0.3">
@@ -51572,9 +51426,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1886" s="5" t="s">
-        <v>3745</v>
-      </c>
       <c r="G1886" s="49"/>
     </row>
     <row r="1887" spans="1:7" x14ac:dyDescent="0.3">
@@ -51595,9 +51446,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1887" s="5" t="s">
-        <v>3747</v>
-      </c>
       <c r="G1887" s="49"/>
     </row>
     <row r="1888" spans="1:7" x14ac:dyDescent="0.3">
@@ -51618,9 +51466,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1888" s="5" t="s">
-        <v>3749</v>
-      </c>
       <c r="G1888" s="49"/>
     </row>
     <row r="1889" spans="1:7" x14ac:dyDescent="0.3">
@@ -51641,9 +51486,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1889" s="5" t="s">
-        <v>3751</v>
-      </c>
       <c r="G1889" s="49"/>
     </row>
     <row r="1890" spans="1:7" x14ac:dyDescent="0.3">
@@ -51664,9 +51506,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1890" s="5" t="s">
-        <v>3753</v>
-      </c>
       <c r="G1890" s="49"/>
     </row>
     <row r="1891" spans="1:7" x14ac:dyDescent="0.3">
@@ -51687,9 +51526,7 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1891" s="5" t="s">
-        <v>3755</v>
-      </c>
+      <c r="F1891"/>
       <c r="G1891" s="49"/>
     </row>
     <row r="1892" spans="1:7" x14ac:dyDescent="0.3">
@@ -51710,9 +51547,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1892" s="5" t="s">
-        <v>3757</v>
-      </c>
       <c r="G1892" s="49"/>
     </row>
     <row r="1893" spans="1:7" x14ac:dyDescent="0.3">
@@ -51733,9 +51567,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1893" s="5" t="s">
-        <v>3759</v>
-      </c>
       <c r="G1893" s="49"/>
     </row>
     <row r="1894" spans="1:7" x14ac:dyDescent="0.3">
@@ -51756,9 +51587,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1894" s="5" t="s">
-        <v>3761</v>
-      </c>
       <c r="G1894" s="49"/>
     </row>
     <row r="1895" spans="1:7" x14ac:dyDescent="0.3">
@@ -51779,9 +51607,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1895" s="5" t="s">
-        <v>3763</v>
-      </c>
       <c r="G1895" s="49"/>
     </row>
     <row r="1896" spans="1:7" x14ac:dyDescent="0.3">
@@ -51802,9 +51627,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1896" s="5" t="s">
-        <v>3765</v>
-      </c>
       <c r="G1896" s="49"/>
     </row>
     <row r="1897" spans="1:7" x14ac:dyDescent="0.3">
@@ -51825,9 +51647,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1897" s="5" t="s">
-        <v>3767</v>
-      </c>
       <c r="G1897" s="49"/>
     </row>
     <row r="1898" spans="1:7" x14ac:dyDescent="0.3">
@@ -51848,9 +51667,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1898" s="5" t="s">
-        <v>3769</v>
-      </c>
       <c r="G1898" s="49"/>
     </row>
     <row r="1899" spans="1:7" x14ac:dyDescent="0.3">
@@ -51871,9 +51687,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1899" s="5" t="s">
-        <v>3771</v>
-      </c>
       <c r="G1899" s="49"/>
     </row>
     <row r="1900" spans="1:7" x14ac:dyDescent="0.3">
@@ -51894,9 +51707,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1900" s="5" t="s">
-        <v>3773</v>
-      </c>
       <c r="G1900" s="49"/>
     </row>
     <row r="1901" spans="1:7" x14ac:dyDescent="0.3">
@@ -51917,9 +51727,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1901" s="5" t="s">
-        <v>3775</v>
-      </c>
       <c r="G1901" s="49"/>
     </row>
     <row r="1902" spans="1:7" x14ac:dyDescent="0.3">
@@ -51940,9 +51747,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1902" s="5" t="s">
-        <v>3777</v>
-      </c>
       <c r="G1902" s="49"/>
     </row>
     <row r="1903" spans="1:7" x14ac:dyDescent="0.3">
@@ -51963,9 +51767,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1903" s="5" t="s">
-        <v>3779</v>
-      </c>
       <c r="G1903" s="49"/>
     </row>
     <row r="1904" spans="1:7" x14ac:dyDescent="0.3">
@@ -51986,9 +51787,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1904" s="5" t="s">
-        <v>3781</v>
-      </c>
       <c r="G1904" s="49"/>
     </row>
     <row r="1905" spans="1:7" x14ac:dyDescent="0.3">
@@ -52009,9 +51807,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1905" s="5" t="s">
-        <v>3783</v>
-      </c>
       <c r="G1905" s="49"/>
     </row>
     <row r="1906" spans="1:7" x14ac:dyDescent="0.3">
@@ -52032,9 +51827,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1906" s="5" t="s">
-        <v>3785</v>
-      </c>
       <c r="G1906" s="49"/>
     </row>
     <row r="1907" spans="1:7" x14ac:dyDescent="0.3">
@@ -52055,9 +51847,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1907" s="5" t="s">
-        <v>3787</v>
-      </c>
       <c r="G1907" s="49"/>
     </row>
     <row r="1908" spans="1:7" x14ac:dyDescent="0.3">
@@ -52078,9 +51867,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1908" s="5" t="s">
-        <v>3789</v>
-      </c>
       <c r="G1908" s="49"/>
     </row>
     <row r="1909" spans="1:7" x14ac:dyDescent="0.3">
@@ -52101,9 +51887,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1909" s="5" t="s">
-        <v>3791</v>
-      </c>
       <c r="G1909" s="49"/>
     </row>
     <row r="1910" spans="1:7" x14ac:dyDescent="0.3">
@@ -52124,9 +51907,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1910" s="5" t="s">
-        <v>3793</v>
-      </c>
       <c r="G1910" s="49"/>
     </row>
     <row r="1911" spans="1:7" x14ac:dyDescent="0.3">
@@ -52147,9 +51927,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1911" s="5" t="s">
-        <v>3795</v>
-      </c>
       <c r="G1911" s="49"/>
     </row>
     <row r="1912" spans="1:7" x14ac:dyDescent="0.3">
@@ -52170,9 +51947,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1912" s="5" t="s">
-        <v>3797</v>
-      </c>
       <c r="G1912" s="49"/>
     </row>
     <row r="1913" spans="1:7" x14ac:dyDescent="0.3">
@@ -52193,9 +51967,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1913" s="5" t="s">
-        <v>3799</v>
-      </c>
       <c r="G1913" s="49"/>
     </row>
     <row r="1914" spans="1:7" x14ac:dyDescent="0.3">
@@ -52216,9 +51987,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1914" s="5" t="s">
-        <v>3801</v>
-      </c>
       <c r="G1914" s="49"/>
     </row>
     <row r="1915" spans="1:7" x14ac:dyDescent="0.3">
@@ -52239,9 +52007,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1915" s="5" t="s">
-        <v>3803</v>
-      </c>
       <c r="G1915" s="49"/>
     </row>
     <row r="1916" spans="1:7" x14ac:dyDescent="0.3">
@@ -52262,9 +52027,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1916" s="5" t="s">
-        <v>3805</v>
-      </c>
       <c r="G1916" s="49"/>
     </row>
     <row r="1917" spans="1:7" x14ac:dyDescent="0.3">
@@ -52285,9 +52047,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1917" s="5" t="s">
-        <v>3807</v>
-      </c>
       <c r="G1917" s="49"/>
     </row>
     <row r="1918" spans="1:7" x14ac:dyDescent="0.3">
@@ -52308,9 +52067,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1918" s="5" t="s">
-        <v>3809</v>
-      </c>
       <c r="G1918" s="49"/>
     </row>
     <row r="1919" spans="1:7" x14ac:dyDescent="0.3">
@@ -52331,9 +52087,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1919" s="5" t="s">
-        <v>3811</v>
-      </c>
       <c r="G1919" s="49"/>
     </row>
     <row r="1920" spans="1:7" x14ac:dyDescent="0.3">
@@ -52354,9 +52107,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1920" s="5" t="s">
-        <v>3813</v>
-      </c>
       <c r="G1920" s="49"/>
     </row>
     <row r="1921" spans="1:7" x14ac:dyDescent="0.3">
@@ -52377,9 +52127,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1921" s="5" t="s">
-        <v>3815</v>
-      </c>
       <c r="G1921" s="49"/>
     </row>
     <row r="1922" spans="1:7" x14ac:dyDescent="0.3">
@@ -52400,9 +52147,6 @@
         <f t="shared" si="59"/>
         <v>12</v>
       </c>
-      <c r="F1922" s="5" t="s">
-        <v>3817</v>
-      </c>
       <c r="G1922" s="49"/>
     </row>
     <row r="1923" spans="1:7" x14ac:dyDescent="0.3">
@@ -52423,9 +52167,6 @@
         <f t="shared" ref="E1923:E1986" si="61">LEN(D1923)</f>
         <v>12</v>
       </c>
-      <c r="F1923" s="5" t="s">
-        <v>3819</v>
-      </c>
       <c r="G1923" s="49"/>
     </row>
     <row r="1924" spans="1:7" x14ac:dyDescent="0.3">
@@ -52446,9 +52187,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1924" s="5" t="s">
-        <v>3821</v>
-      </c>
       <c r="G1924" s="49"/>
     </row>
     <row r="1925" spans="1:7" x14ac:dyDescent="0.3">
@@ -52469,9 +52207,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1925" s="5" t="s">
-        <v>3823</v>
-      </c>
       <c r="G1925" s="49"/>
     </row>
     <row r="1926" spans="1:7" x14ac:dyDescent="0.3">
@@ -52492,9 +52227,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1926" s="5" t="s">
-        <v>3825</v>
-      </c>
       <c r="G1926" s="49"/>
     </row>
     <row r="1927" spans="1:7" x14ac:dyDescent="0.3">
@@ -52515,9 +52247,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1927" s="5" t="s">
-        <v>3827</v>
-      </c>
       <c r="G1927" s="49"/>
     </row>
     <row r="1928" spans="1:7" x14ac:dyDescent="0.3">
@@ -52538,9 +52267,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1928" s="5" t="s">
-        <v>3829</v>
-      </c>
       <c r="G1928" s="49"/>
     </row>
     <row r="1929" spans="1:7" x14ac:dyDescent="0.3">
@@ -52561,9 +52287,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1929" s="5" t="s">
-        <v>3831</v>
-      </c>
       <c r="G1929" s="49"/>
     </row>
     <row r="1930" spans="1:7" x14ac:dyDescent="0.3">
@@ -52584,9 +52307,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1930" s="5" t="s">
-        <v>3833</v>
-      </c>
       <c r="G1930" s="49"/>
     </row>
     <row r="1931" spans="1:7" x14ac:dyDescent="0.3">
@@ -52607,9 +52327,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1931" s="5" t="s">
-        <v>3835</v>
-      </c>
       <c r="G1931" s="49"/>
     </row>
     <row r="1932" spans="1:7" x14ac:dyDescent="0.3">
@@ -52630,9 +52347,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1932" s="5" t="s">
-        <v>3837</v>
-      </c>
       <c r="G1932" s="49"/>
     </row>
     <row r="1933" spans="1:7" x14ac:dyDescent="0.3">
@@ -52653,9 +52367,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1933" s="5" t="s">
-        <v>3839</v>
-      </c>
       <c r="G1933" s="49"/>
     </row>
     <row r="1934" spans="1:7" x14ac:dyDescent="0.3">
@@ -52676,9 +52387,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1934" s="5" t="s">
-        <v>3841</v>
-      </c>
       <c r="G1934" s="49"/>
     </row>
     <row r="1935" spans="1:7" x14ac:dyDescent="0.3">
@@ -52699,9 +52407,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1935" s="5" t="s">
-        <v>3843</v>
-      </c>
       <c r="G1935" s="49"/>
     </row>
     <row r="1936" spans="1:7" x14ac:dyDescent="0.3">
@@ -52722,9 +52427,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1936" s="5" t="s">
-        <v>3845</v>
-      </c>
       <c r="G1936" s="49"/>
     </row>
     <row r="1937" spans="1:7" x14ac:dyDescent="0.3">
@@ -52745,9 +52447,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1937" s="5" t="s">
-        <v>3847</v>
-      </c>
       <c r="G1937" s="49"/>
     </row>
     <row r="1938" spans="1:7" x14ac:dyDescent="0.3">
@@ -52768,9 +52467,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1938" s="5" t="s">
-        <v>3849</v>
-      </c>
       <c r="G1938" s="49"/>
     </row>
     <row r="1939" spans="1:7" x14ac:dyDescent="0.3">
@@ -52791,9 +52487,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1939" s="5" t="s">
-        <v>3851</v>
-      </c>
       <c r="G1939" s="49"/>
     </row>
     <row r="1940" spans="1:7" x14ac:dyDescent="0.3">
@@ -52814,9 +52507,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1940" s="5" t="s">
-        <v>3853</v>
-      </c>
       <c r="G1940" s="49"/>
     </row>
     <row r="1941" spans="1:7" x14ac:dyDescent="0.3">
@@ -52837,9 +52527,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1941" s="5" t="s">
-        <v>3855</v>
-      </c>
       <c r="G1941" s="49"/>
     </row>
     <row r="1942" spans="1:7" x14ac:dyDescent="0.3">
@@ -52860,9 +52547,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1942" s="5" t="s">
-        <v>3857</v>
-      </c>
       <c r="G1942" s="49"/>
     </row>
     <row r="1943" spans="1:7" x14ac:dyDescent="0.3">
@@ -52883,9 +52567,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1943" s="5" t="s">
-        <v>3859</v>
-      </c>
       <c r="G1943" s="49"/>
     </row>
     <row r="1944" spans="1:7" x14ac:dyDescent="0.3">
@@ -52906,9 +52587,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1944" s="5" t="s">
-        <v>3861</v>
-      </c>
       <c r="G1944" s="49"/>
     </row>
     <row r="1945" spans="1:7" x14ac:dyDescent="0.3">
@@ -52929,9 +52607,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1945" s="5" t="s">
-        <v>3863</v>
-      </c>
       <c r="G1945" s="49"/>
     </row>
     <row r="1946" spans="1:7" x14ac:dyDescent="0.3">
@@ -52952,9 +52627,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1946" s="5" t="s">
-        <v>3865</v>
-      </c>
       <c r="G1946" s="49"/>
     </row>
     <row r="1947" spans="1:7" x14ac:dyDescent="0.3">
@@ -52975,9 +52647,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1947" s="5" t="s">
-        <v>3867</v>
-      </c>
       <c r="G1947" s="49"/>
     </row>
     <row r="1948" spans="1:7" x14ac:dyDescent="0.3">
@@ -52998,9 +52667,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1948" s="5" t="s">
-        <v>3869</v>
-      </c>
       <c r="G1948" s="49"/>
     </row>
     <row r="1949" spans="1:7" x14ac:dyDescent="0.3">
@@ -53021,9 +52687,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1949" s="5" t="s">
-        <v>3871</v>
-      </c>
       <c r="G1949" s="49"/>
     </row>
     <row r="1950" spans="1:7" x14ac:dyDescent="0.3">
@@ -53044,9 +52707,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1950" s="5" t="s">
-        <v>3873</v>
-      </c>
       <c r="G1950" s="49"/>
     </row>
     <row r="1951" spans="1:7" x14ac:dyDescent="0.3">
@@ -53067,9 +52727,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1951" s="5" t="s">
-        <v>3875</v>
-      </c>
       <c r="G1951" s="49"/>
     </row>
     <row r="1952" spans="1:7" x14ac:dyDescent="0.3">
@@ -53090,9 +52747,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1952" s="5" t="s">
-        <v>3877</v>
-      </c>
       <c r="G1952" s="49"/>
     </row>
     <row r="1953" spans="1:7" x14ac:dyDescent="0.3">
@@ -53113,9 +52767,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1953" s="5" t="s">
-        <v>3879</v>
-      </c>
       <c r="G1953" s="49"/>
     </row>
     <row r="1954" spans="1:7" x14ac:dyDescent="0.3">
@@ -53136,9 +52787,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1954" s="5" t="s">
-        <v>3881</v>
-      </c>
       <c r="G1954" s="49"/>
     </row>
     <row r="1955" spans="1:7" x14ac:dyDescent="0.3">
@@ -53159,9 +52807,7 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1955" s="5" t="s">
-        <v>3883</v>
-      </c>
+      <c r="F1955"/>
       <c r="G1955" s="49"/>
     </row>
     <row r="1956" spans="1:7" x14ac:dyDescent="0.3">
@@ -53182,9 +52828,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1956" s="5" t="s">
-        <v>3885</v>
-      </c>
       <c r="G1956" s="49"/>
     </row>
     <row r="1957" spans="1:7" x14ac:dyDescent="0.3">
@@ -53205,9 +52848,7 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1957" s="5" t="s">
-        <v>3887</v>
-      </c>
+      <c r="F1957"/>
       <c r="G1957" s="49"/>
     </row>
     <row r="1958" spans="1:7" x14ac:dyDescent="0.3">
@@ -53228,9 +52869,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1958" s="5" t="s">
-        <v>3889</v>
-      </c>
       <c r="G1958" s="49"/>
     </row>
     <row r="1959" spans="1:7" x14ac:dyDescent="0.3">
@@ -53251,9 +52889,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1959" s="5" t="s">
-        <v>3891</v>
-      </c>
       <c r="G1959" s="49"/>
     </row>
     <row r="1960" spans="1:7" x14ac:dyDescent="0.3">
@@ -53274,9 +52909,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1960" s="5" t="s">
-        <v>3893</v>
-      </c>
       <c r="G1960" s="49"/>
     </row>
     <row r="1961" spans="1:7" x14ac:dyDescent="0.3">
@@ -53297,9 +52929,7 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1961" s="5" t="s">
-        <v>3895</v>
-      </c>
+      <c r="F1961"/>
       <c r="G1961" s="49"/>
     </row>
     <row r="1962" spans="1:7" x14ac:dyDescent="0.3">
@@ -53320,9 +52950,7 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1962" s="5" t="s">
-        <v>3897</v>
-      </c>
+      <c r="F1962"/>
       <c r="G1962" s="49"/>
     </row>
     <row r="1963" spans="1:7" x14ac:dyDescent="0.3">
@@ -53343,9 +52971,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1963" s="5" t="s">
-        <v>3899</v>
-      </c>
       <c r="G1963" s="49"/>
     </row>
     <row r="1964" spans="1:7" x14ac:dyDescent="0.3">
@@ -53366,9 +52991,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1964" s="5" t="s">
-        <v>3901</v>
-      </c>
       <c r="G1964" s="49"/>
     </row>
     <row r="1965" spans="1:7" x14ac:dyDescent="0.3">
@@ -53389,9 +53011,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1965" s="5" t="s">
-        <v>3903</v>
-      </c>
       <c r="G1965" s="49"/>
     </row>
     <row r="1966" spans="1:7" x14ac:dyDescent="0.3">
@@ -53412,9 +53031,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1966" s="5" t="s">
-        <v>3905</v>
-      </c>
       <c r="G1966" s="49"/>
     </row>
     <row r="1967" spans="1:7" x14ac:dyDescent="0.3">
@@ -53435,9 +53051,7 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1967" s="5" t="s">
-        <v>3907</v>
-      </c>
+      <c r="F1967"/>
       <c r="G1967" s="49"/>
     </row>
     <row r="1968" spans="1:7" x14ac:dyDescent="0.3">
@@ -53458,9 +53072,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1968" s="5" t="s">
-        <v>3909</v>
-      </c>
       <c r="G1968" s="49"/>
     </row>
     <row r="1969" spans="1:7" x14ac:dyDescent="0.3">
@@ -53481,9 +53092,6 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1969" s="5" t="s">
-        <v>3911</v>
-      </c>
       <c r="G1969" s="49"/>
     </row>
     <row r="1970" spans="1:7" x14ac:dyDescent="0.3">
@@ -53504,9 +53112,7 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1970" s="5" t="s">
-        <v>3913</v>
-      </c>
+      <c r="F1970"/>
       <c r="G1970" s="49"/>
     </row>
     <row r="1971" spans="1:7" x14ac:dyDescent="0.3">
@@ -53527,9 +53133,7 @@
         <f t="shared" si="61"/>
         <v>12</v>
       </c>
-      <c r="F1971" s="5" t="s">
-        <v>3915</v>
-      </c>
+      <c r="F1971"/>
       <c r="G1971" s="49"/>
     </row>
     <row r="1972" spans="1:7" x14ac:dyDescent="0.3">
@@ -53850,9 +53454,7 @@
         <f t="shared" ref="E1987:E2050" si="63">LEN(D1987)</f>
         <v>12</v>
       </c>
-      <c r="F1987" t="s">
-        <v>3947</v>
-      </c>
+      <c r="F1987"/>
       <c r="G1987" s="49"/>
     </row>
     <row r="1988" spans="1:7" x14ac:dyDescent="0.3">
@@ -54173,9 +53775,7 @@
         <f t="shared" si="63"/>
         <v>12</v>
       </c>
-      <c r="F2003" t="s">
-        <v>3979</v>
-      </c>
+      <c r="F2003"/>
       <c r="G2003" s="49"/>
     </row>
     <row r="2004" spans="1:7" x14ac:dyDescent="0.3">
@@ -55266,8 +54866,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="67"/>
-      <c r="B3" s="64" t="str">
+      <c r="A3" s="64"/>
+      <c r="B3" s="66" t="str">
         <f>CONCATENATE(A3,A7,A11,A15)</f>
         <v/>
       </c>
@@ -55280,8 +54880,8 @@
         <v>6</v>
       </c>
       <c r="G3" s="18"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="64" t="str">
+      <c r="H3" s="64"/>
+      <c r="I3" s="66" t="str">
         <f>CONCATENATE(H3,H7,H11,H15)</f>
         <v/>
       </c>
@@ -55294,8 +54894,8 @@
         <v>6</v>
       </c>
       <c r="N3" s="18"/>
-      <c r="O3" s="67"/>
-      <c r="P3" s="64" t="str">
+      <c r="O3" s="64"/>
+      <c r="P3" s="66" t="str">
         <f>CONCATENATE(O3,O7,O11,O15)</f>
         <v/>
       </c>
@@ -55405,7 +55005,7 @@
       </c>
     </row>
     <row r="7" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="67"/>
+      <c r="A7" s="64"/>
       <c r="B7" s="65"/>
       <c r="C7" s="40"/>
       <c r="D7" s="48"/>
@@ -55415,7 +55015,7 @@
       <c r="F7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="67"/>
+      <c r="H7" s="64"/>
       <c r="I7" s="65"/>
       <c r="J7" s="36"/>
       <c r="K7" s="35"/>
@@ -55425,7 +55025,7 @@
       <c r="M7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O7" s="67"/>
+      <c r="O7" s="64"/>
       <c r="P7" s="65"/>
       <c r="Q7" s="36"/>
       <c r="R7" s="35"/>
@@ -55533,7 +55133,7 @@
       </c>
     </row>
     <row r="11" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="67"/>
+      <c r="A11" s="64"/>
       <c r="B11" s="65"/>
       <c r="C11" s="40"/>
       <c r="D11" s="48"/>
@@ -55543,7 +55143,7 @@
       <c r="F11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="67"/>
+      <c r="H11" s="64"/>
       <c r="I11" s="65"/>
       <c r="J11" s="36"/>
       <c r="K11" s="35"/>
@@ -55553,7 +55153,7 @@
       <c r="M11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O11" s="67"/>
+      <c r="O11" s="64"/>
       <c r="P11" s="65"/>
       <c r="Q11" s="36"/>
       <c r="R11" s="35"/>
@@ -55661,7 +55261,7 @@
       </c>
     </row>
     <row r="15" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="67"/>
+      <c r="A15" s="64"/>
       <c r="B15" s="65"/>
       <c r="C15" s="47"/>
       <c r="D15" s="43"/>
@@ -55671,7 +55271,7 @@
       <c r="F15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="67"/>
+      <c r="H15" s="64"/>
       <c r="I15" s="65"/>
       <c r="J15" s="36"/>
       <c r="K15" s="35"/>
@@ -55681,7 +55281,7 @@
       <c r="M15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="O15" s="67"/>
+      <c r="O15" s="64"/>
       <c r="P15" s="65"/>
       <c r="Q15" s="36"/>
       <c r="R15" s="35"/>
@@ -55791,8 +55391,8 @@
       </c>
     </row>
     <row r="19" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="67"/>
-      <c r="B19" s="64" t="str">
+      <c r="A19" s="64"/>
+      <c r="B19" s="66" t="str">
         <f>CONCATENATE(A19,A23,A27,A31)</f>
         <v/>
       </c>
@@ -55805,8 +55405,8 @@
         <v>38</v>
       </c>
       <c r="G19" s="18"/>
-      <c r="H19" s="67"/>
-      <c r="I19" s="64" t="str">
+      <c r="H19" s="64"/>
+      <c r="I19" s="66" t="str">
         <f>CONCATENATE(H19,H23,H27,H31)</f>
         <v/>
       </c>
@@ -55819,8 +55419,8 @@
         <v>38</v>
       </c>
       <c r="N19" s="18"/>
-      <c r="O19" s="67"/>
-      <c r="P19" s="64" t="str">
+      <c r="O19" s="64"/>
+      <c r="P19" s="66" t="str">
         <f>CONCATENATE(O19,O23,O27,O31)</f>
         <v/>
       </c>
@@ -55930,7 +55530,7 @@
       </c>
     </row>
     <row r="23" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="67"/>
+      <c r="A23" s="64"/>
       <c r="B23" s="65"/>
       <c r="C23" s="25"/>
       <c r="D23" s="35"/>
@@ -55940,7 +55540,7 @@
       <c r="F23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H23" s="67"/>
+      <c r="H23" s="64"/>
       <c r="I23" s="65"/>
       <c r="J23" s="36"/>
       <c r="K23" s="35"/>
@@ -55950,7 +55550,7 @@
       <c r="M23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="O23" s="67"/>
+      <c r="O23" s="64"/>
       <c r="P23" s="65"/>
       <c r="Q23" s="25"/>
       <c r="R23" s="35"/>
@@ -56058,7 +55658,7 @@
       </c>
     </row>
     <row r="27" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="67"/>
+      <c r="A27" s="64"/>
       <c r="B27" s="65"/>
       <c r="C27" s="25"/>
       <c r="D27" s="35"/>
@@ -56068,7 +55668,7 @@
       <c r="F27" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H27" s="67"/>
+      <c r="H27" s="64"/>
       <c r="I27" s="65"/>
       <c r="J27" s="36"/>
       <c r="K27" s="35"/>
@@ -56078,7 +55678,7 @@
       <c r="M27" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="O27" s="67"/>
+      <c r="O27" s="64"/>
       <c r="P27" s="65"/>
       <c r="Q27" s="25"/>
       <c r="R27" s="35"/>
@@ -56186,7 +55786,7 @@
       </c>
     </row>
     <row r="31" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="67"/>
+      <c r="A31" s="64"/>
       <c r="B31" s="65"/>
       <c r="C31" s="25"/>
       <c r="D31" s="35"/>
@@ -56196,7 +55796,7 @@
       <c r="F31" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H31" s="67"/>
+      <c r="H31" s="64"/>
       <c r="I31" s="65"/>
       <c r="J31" s="36"/>
       <c r="K31" s="35"/>
@@ -56206,7 +55806,7 @@
       <c r="M31" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="O31" s="67"/>
+      <c r="O31" s="64"/>
       <c r="P31" s="65"/>
       <c r="Q31" s="25"/>
       <c r="R31" s="35"/>
@@ -56316,8 +55916,8 @@
       </c>
     </row>
     <row r="35" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="67"/>
-      <c r="B35" s="64" t="str">
+      <c r="A35" s="64"/>
+      <c r="B35" s="66" t="str">
         <f>CONCATENATE(A35,A39,A43,A47)</f>
         <v/>
       </c>
@@ -56330,8 +55930,8 @@
         <v>70</v>
       </c>
       <c r="G35" s="18"/>
-      <c r="H35" s="67"/>
-      <c r="I35" s="64" t="str">
+      <c r="H35" s="64"/>
+      <c r="I35" s="66" t="str">
         <f>CONCATENATE(H35,H39,H43,H47)</f>
         <v/>
       </c>
@@ -56344,8 +55944,8 @@
         <v>70</v>
       </c>
       <c r="N35" s="18"/>
-      <c r="O35" s="67"/>
-      <c r="P35" s="64" t="str">
+      <c r="O35" s="64"/>
+      <c r="P35" s="66" t="str">
         <f>CONCATENATE(O35,O39,O43,O47)</f>
         <v/>
       </c>
@@ -56455,7 +56055,7 @@
       </c>
     </row>
     <row r="39" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="67"/>
+      <c r="A39" s="64"/>
       <c r="B39" s="65"/>
       <c r="C39" s="25"/>
       <c r="D39" s="35"/>
@@ -56465,7 +56065,7 @@
       <c r="F39" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H39" s="67"/>
+      <c r="H39" s="64"/>
       <c r="I39" s="65"/>
       <c r="J39" s="36"/>
       <c r="K39" s="35"/>
@@ -56475,7 +56075,7 @@
       <c r="M39" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="O39" s="67"/>
+      <c r="O39" s="64"/>
       <c r="P39" s="65"/>
       <c r="Q39" s="25"/>
       <c r="R39" s="35"/>
@@ -56583,7 +56183,7 @@
       </c>
     </row>
     <row r="43" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="67"/>
+      <c r="A43" s="64"/>
       <c r="B43" s="65"/>
       <c r="C43" s="25"/>
       <c r="D43" s="35"/>
@@ -56593,7 +56193,7 @@
       <c r="F43" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H43" s="67"/>
+      <c r="H43" s="64"/>
       <c r="I43" s="65"/>
       <c r="J43" s="36"/>
       <c r="K43" s="35"/>
@@ -56603,7 +56203,7 @@
       <c r="M43" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="O43" s="67"/>
+      <c r="O43" s="64"/>
       <c r="P43" s="65"/>
       <c r="Q43" s="25"/>
       <c r="R43" s="35"/>
@@ -56711,7 +56311,7 @@
       </c>
     </row>
     <row r="47" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="67"/>
+      <c r="A47" s="64"/>
       <c r="B47" s="65"/>
       <c r="C47" s="25"/>
       <c r="D47" s="35"/>
@@ -56721,7 +56321,7 @@
       <c r="F47" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="H47" s="67"/>
+      <c r="H47" s="64"/>
       <c r="I47" s="65"/>
       <c r="J47" s="36"/>
       <c r="K47" s="35"/>
@@ -56731,7 +56331,7 @@
       <c r="M47" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="O47" s="67"/>
+      <c r="O47" s="64"/>
       <c r="P47" s="65"/>
       <c r="Q47" s="25"/>
       <c r="R47" s="35"/>
@@ -56841,8 +56441,8 @@
       </c>
     </row>
     <row r="51" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="67"/>
-      <c r="B51" s="64" t="str">
+      <c r="A51" s="64"/>
+      <c r="B51" s="66" t="str">
         <f>CONCATENATE(A51,A55,A59,A63)</f>
         <v/>
       </c>
@@ -56855,8 +56455,8 @@
         <v>102</v>
       </c>
       <c r="G51" s="18"/>
-      <c r="H51" s="67"/>
-      <c r="I51" s="64" t="str">
+      <c r="H51" s="64"/>
+      <c r="I51" s="66" t="str">
         <f>CONCATENATE(H51,H55,H59,H63)</f>
         <v/>
       </c>
@@ -56869,8 +56469,8 @@
         <v>102</v>
       </c>
       <c r="N51" s="18"/>
-      <c r="O51" s="67"/>
-      <c r="P51" s="64" t="str">
+      <c r="O51" s="64"/>
+      <c r="P51" s="66" t="str">
         <f>CONCATENATE(O51,O55,O59,O63)</f>
         <v/>
       </c>
@@ -56980,7 +56580,7 @@
       </c>
     </row>
     <row r="55" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="67"/>
+      <c r="A55" s="64"/>
       <c r="B55" s="65"/>
       <c r="C55" s="25"/>
       <c r="D55" s="35"/>
@@ -56990,7 +56590,7 @@
       <c r="F55" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="H55" s="67"/>
+      <c r="H55" s="64"/>
       <c r="I55" s="65"/>
       <c r="J55" s="36"/>
       <c r="K55" s="35"/>
@@ -57000,7 +56600,7 @@
       <c r="M55" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="O55" s="67"/>
+      <c r="O55" s="64"/>
       <c r="P55" s="65"/>
       <c r="Q55" s="25"/>
       <c r="R55" s="35"/>
@@ -57108,7 +56708,7 @@
       </c>
     </row>
     <row r="59" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="67"/>
+      <c r="A59" s="64"/>
       <c r="B59" s="65"/>
       <c r="C59" s="25"/>
       <c r="D59" s="35"/>
@@ -57118,7 +56718,7 @@
       <c r="F59" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="H59" s="67"/>
+      <c r="H59" s="64"/>
       <c r="I59" s="65"/>
       <c r="J59" s="36"/>
       <c r="K59" s="35"/>
@@ -57128,7 +56728,7 @@
       <c r="M59" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="O59" s="67"/>
+      <c r="O59" s="64"/>
       <c r="P59" s="65"/>
       <c r="Q59" s="25"/>
       <c r="R59" s="35"/>
@@ -57236,7 +56836,7 @@
       </c>
     </row>
     <row r="63" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="67"/>
+      <c r="A63" s="64"/>
       <c r="B63" s="65"/>
       <c r="C63" s="25"/>
       <c r="D63" s="35"/>
@@ -57246,7 +56846,7 @@
       <c r="F63" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="H63" s="67"/>
+      <c r="H63" s="64"/>
       <c r="I63" s="65"/>
       <c r="J63" s="36"/>
       <c r="K63" s="35"/>
@@ -57256,7 +56856,7 @@
       <c r="M63" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="O63" s="67"/>
+      <c r="O63" s="64"/>
       <c r="P63" s="65"/>
       <c r="Q63" s="25"/>
       <c r="R63" s="35"/>
@@ -57366,8 +56966,8 @@
       </c>
     </row>
     <row r="67" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="67"/>
-      <c r="B67" s="64" t="str">
+      <c r="A67" s="64"/>
+      <c r="B67" s="66" t="str">
         <f>CONCATENATE(A67,A71,A75,A79)</f>
         <v/>
       </c>
@@ -57380,8 +56980,8 @@
         <v>134</v>
       </c>
       <c r="G67" s="18"/>
-      <c r="H67" s="67"/>
-      <c r="I67" s="64" t="str">
+      <c r="H67" s="64"/>
+      <c r="I67" s="66" t="str">
         <f>CONCATENATE(H67,H71,H75,H79)</f>
         <v/>
       </c>
@@ -57394,8 +56994,8 @@
         <v>134</v>
       </c>
       <c r="N67" s="18"/>
-      <c r="O67" s="67"/>
-      <c r="P67" s="64" t="str">
+      <c r="O67" s="64"/>
+      <c r="P67" s="66" t="str">
         <f>CONCATENATE(O67,O71,O75,O79)</f>
         <v/>
       </c>
@@ -57505,7 +57105,7 @@
       </c>
     </row>
     <row r="71" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="67"/>
+      <c r="A71" s="64"/>
       <c r="B71" s="65"/>
       <c r="C71" s="25"/>
       <c r="D71" s="35"/>
@@ -57515,7 +57115,7 @@
       <c r="F71" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="H71" s="67"/>
+      <c r="H71" s="64"/>
       <c r="I71" s="65"/>
       <c r="J71" s="36"/>
       <c r="K71" s="35"/>
@@ -57525,7 +57125,7 @@
       <c r="M71" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="O71" s="67"/>
+      <c r="O71" s="64"/>
       <c r="P71" s="65"/>
       <c r="Q71" s="25"/>
       <c r="R71" s="35"/>
@@ -57633,7 +57233,7 @@
       </c>
     </row>
     <row r="75" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="67"/>
+      <c r="A75" s="64"/>
       <c r="B75" s="65"/>
       <c r="C75" s="25"/>
       <c r="D75" s="35"/>
@@ -57643,7 +57243,7 @@
       <c r="F75" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="H75" s="67"/>
+      <c r="H75" s="64"/>
       <c r="I75" s="65"/>
       <c r="J75" s="36"/>
       <c r="K75" s="35"/>
@@ -57653,7 +57253,7 @@
       <c r="M75" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="O75" s="67"/>
+      <c r="O75" s="64"/>
       <c r="P75" s="65"/>
       <c r="Q75" s="25"/>
       <c r="R75" s="35"/>
@@ -57761,7 +57361,7 @@
       </c>
     </row>
     <row r="79" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="67"/>
+      <c r="A79" s="64"/>
       <c r="B79" s="65"/>
       <c r="C79" s="25"/>
       <c r="D79" s="35"/>
@@ -57771,7 +57371,7 @@
       <c r="F79" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="H79" s="67"/>
+      <c r="H79" s="64"/>
       <c r="I79" s="65"/>
       <c r="J79" s="36"/>
       <c r="K79" s="35"/>
@@ -57781,7 +57381,7 @@
       <c r="M79" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="O79" s="67"/>
+      <c r="O79" s="64"/>
       <c r="P79" s="65"/>
       <c r="Q79" s="25"/>
       <c r="R79" s="35"/>
@@ -57891,8 +57491,8 @@
       </c>
     </row>
     <row r="83" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="67"/>
-      <c r="B83" s="64" t="str">
+      <c r="A83" s="64"/>
+      <c r="B83" s="66" t="str">
         <f>CONCATENATE(A83,A87,A91,A95)</f>
         <v/>
       </c>
@@ -57905,8 +57505,8 @@
         <v>166</v>
       </c>
       <c r="G83" s="18"/>
-      <c r="H83" s="67"/>
-      <c r="I83" s="64" t="str">
+      <c r="H83" s="64"/>
+      <c r="I83" s="66" t="str">
         <f>CONCATENATE(H83,H87,H91,H95)</f>
         <v/>
       </c>
@@ -57919,8 +57519,8 @@
         <v>166</v>
       </c>
       <c r="N83" s="18"/>
-      <c r="O83" s="67"/>
-      <c r="P83" s="64" t="str">
+      <c r="O83" s="64"/>
+      <c r="P83" s="66" t="str">
         <f>CONCATENATE(O83,O87,O91,O95)</f>
         <v/>
       </c>
@@ -58030,7 +57630,7 @@
       </c>
     </row>
     <row r="87" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="67"/>
+      <c r="A87" s="64"/>
       <c r="B87" s="65"/>
       <c r="C87" s="25"/>
       <c r="D87" s="35"/>
@@ -58040,7 +57640,7 @@
       <c r="F87" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="H87" s="67"/>
+      <c r="H87" s="64"/>
       <c r="I87" s="65"/>
       <c r="J87" s="36"/>
       <c r="K87" s="35"/>
@@ -58050,7 +57650,7 @@
       <c r="M87" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="O87" s="67"/>
+      <c r="O87" s="64"/>
       <c r="P87" s="65"/>
       <c r="Q87" s="25"/>
       <c r="R87" s="35"/>
@@ -58158,7 +57758,7 @@
       </c>
     </row>
     <row r="91" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="67"/>
+      <c r="A91" s="64"/>
       <c r="B91" s="65"/>
       <c r="C91" s="25"/>
       <c r="D91" s="35"/>
@@ -58168,7 +57768,7 @@
       <c r="F91" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="H91" s="67"/>
+      <c r="H91" s="64"/>
       <c r="I91" s="65"/>
       <c r="J91" s="36"/>
       <c r="K91" s="35"/>
@@ -58178,7 +57778,7 @@
       <c r="M91" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="O91" s="67"/>
+      <c r="O91" s="64"/>
       <c r="P91" s="65"/>
       <c r="Q91" s="25"/>
       <c r="R91" s="35"/>
@@ -58286,7 +57886,7 @@
       </c>
     </row>
     <row r="95" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="67"/>
+      <c r="A95" s="64"/>
       <c r="B95" s="65"/>
       <c r="C95" s="25"/>
       <c r="D95" s="35"/>
@@ -58296,7 +57896,7 @@
       <c r="F95" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="H95" s="67"/>
+      <c r="H95" s="64"/>
       <c r="I95" s="65"/>
       <c r="J95" s="36"/>
       <c r="K95" s="35"/>
@@ -58306,7 +57906,7 @@
       <c r="M95" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="O95" s="67"/>
+      <c r="O95" s="64"/>
       <c r="P95" s="65"/>
       <c r="Q95" s="25"/>
       <c r="R95" s="35"/>
@@ -58416,8 +58016,8 @@
       </c>
     </row>
     <row r="99" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="67"/>
-      <c r="B99" s="64" t="str">
+      <c r="A99" s="64"/>
+      <c r="B99" s="66" t="str">
         <f>CONCATENATE(A99,A103,A107,A111)</f>
         <v/>
       </c>
@@ -58430,8 +58030,8 @@
         <v>198</v>
       </c>
       <c r="G99" s="18"/>
-      <c r="H99" s="67"/>
-      <c r="I99" s="64" t="str">
+      <c r="H99" s="64"/>
+      <c r="I99" s="66" t="str">
         <f>CONCATENATE(H99,H103,H107,H111)</f>
         <v/>
       </c>
@@ -58444,8 +58044,8 @@
         <v>198</v>
       </c>
       <c r="N99" s="18"/>
-      <c r="O99" s="67"/>
-      <c r="P99" s="64" t="str">
+      <c r="O99" s="64"/>
+      <c r="P99" s="66" t="str">
         <f>CONCATENATE(O99,O103,O107,O111)</f>
         <v/>
       </c>
@@ -58555,7 +58155,7 @@
       </c>
     </row>
     <row r="103" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="67"/>
+      <c r="A103" s="64"/>
       <c r="B103" s="65"/>
       <c r="C103" s="25"/>
       <c r="D103" s="35"/>
@@ -58565,7 +58165,7 @@
       <c r="F103" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="H103" s="67"/>
+      <c r="H103" s="64"/>
       <c r="I103" s="65"/>
       <c r="J103" s="36"/>
       <c r="K103" s="35"/>
@@ -58575,7 +58175,7 @@
       <c r="M103" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="O103" s="67"/>
+      <c r="O103" s="64"/>
       <c r="P103" s="65"/>
       <c r="Q103" s="25"/>
       <c r="R103" s="35"/>
@@ -58683,7 +58283,7 @@
       </c>
     </row>
     <row r="107" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="67"/>
+      <c r="A107" s="64"/>
       <c r="B107" s="65"/>
       <c r="C107" s="25"/>
       <c r="D107" s="35"/>
@@ -58693,7 +58293,7 @@
       <c r="F107" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="H107" s="67"/>
+      <c r="H107" s="64"/>
       <c r="I107" s="65"/>
       <c r="J107" s="36"/>
       <c r="K107" s="35"/>
@@ -58703,7 +58303,7 @@
       <c r="M107" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="O107" s="67"/>
+      <c r="O107" s="64"/>
       <c r="P107" s="65"/>
       <c r="Q107" s="25"/>
       <c r="R107" s="35"/>
@@ -58811,7 +58411,7 @@
       </c>
     </row>
     <row r="111" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="67"/>
+      <c r="A111" s="64"/>
       <c r="B111" s="65"/>
       <c r="C111" s="25"/>
       <c r="D111" s="35"/>
@@ -58821,7 +58421,7 @@
       <c r="F111" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="H111" s="67"/>
+      <c r="H111" s="64"/>
       <c r="I111" s="65"/>
       <c r="J111" s="36"/>
       <c r="K111" s="35"/>
@@ -58831,7 +58431,7 @@
       <c r="M111" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="O111" s="67"/>
+      <c r="O111" s="64"/>
       <c r="P111" s="65"/>
       <c r="Q111" s="25"/>
       <c r="R111" s="35"/>
@@ -58941,8 +58541,8 @@
       </c>
     </row>
     <row r="115" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="67"/>
-      <c r="B115" s="64" t="str">
+      <c r="A115" s="64"/>
+      <c r="B115" s="66" t="str">
         <f>CONCATENATE(A115,A119,A123,A127)</f>
         <v/>
       </c>
@@ -58955,8 +58555,8 @@
         <v>230</v>
       </c>
       <c r="G115" s="18"/>
-      <c r="H115" s="67"/>
-      <c r="I115" s="64" t="str">
+      <c r="H115" s="64"/>
+      <c r="I115" s="66" t="str">
         <f>CONCATENATE(H115,H119,H123,H127)</f>
         <v/>
       </c>
@@ -58969,8 +58569,8 @@
         <v>230</v>
       </c>
       <c r="N115" s="18"/>
-      <c r="O115" s="67"/>
-      <c r="P115" s="64" t="str">
+      <c r="O115" s="64"/>
+      <c r="P115" s="66" t="str">
         <f>CONCATENATE(O115,O119,O123,O127)</f>
         <v/>
       </c>
@@ -59080,7 +58680,7 @@
       </c>
     </row>
     <row r="119" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="67"/>
+      <c r="A119" s="64"/>
       <c r="B119" s="65"/>
       <c r="C119" s="25"/>
       <c r="D119" s="35"/>
@@ -59090,7 +58690,7 @@
       <c r="F119" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="H119" s="67"/>
+      <c r="H119" s="64"/>
       <c r="I119" s="65"/>
       <c r="J119" s="36"/>
       <c r="K119" s="35"/>
@@ -59100,7 +58700,7 @@
       <c r="M119" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="O119" s="67"/>
+      <c r="O119" s="64"/>
       <c r="P119" s="65"/>
       <c r="Q119" s="25"/>
       <c r="R119" s="35"/>
@@ -59208,7 +58808,7 @@
       </c>
     </row>
     <row r="123" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="67"/>
+      <c r="A123" s="64"/>
       <c r="B123" s="65"/>
       <c r="C123" s="25"/>
       <c r="D123" s="35"/>
@@ -59218,7 +58818,7 @@
       <c r="F123" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="H123" s="67"/>
+      <c r="H123" s="64"/>
       <c r="I123" s="65"/>
       <c r="J123" s="36"/>
       <c r="K123" s="35"/>
@@ -59228,7 +58828,7 @@
       <c r="M123" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="O123" s="67"/>
+      <c r="O123" s="64"/>
       <c r="P123" s="65"/>
       <c r="Q123" s="25"/>
       <c r="R123" s="35"/>
@@ -59336,7 +58936,7 @@
       </c>
     </row>
     <row r="127" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="67"/>
+      <c r="A127" s="64"/>
       <c r="B127" s="65"/>
       <c r="C127" s="25"/>
       <c r="D127" s="35"/>
@@ -59346,7 +58946,7 @@
       <c r="F127" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="H127" s="67"/>
+      <c r="H127" s="64"/>
       <c r="I127" s="65"/>
       <c r="J127" s="36"/>
       <c r="K127" s="35"/>
@@ -59356,7 +58956,7 @@
       <c r="M127" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="O127" s="67"/>
+      <c r="O127" s="64"/>
       <c r="P127" s="65"/>
       <c r="Q127" s="25"/>
       <c r="R127" s="35"/>
@@ -59466,8 +59066,8 @@
       </c>
     </row>
     <row r="131" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="67"/>
-      <c r="B131" s="64" t="str">
+      <c r="A131" s="64"/>
+      <c r="B131" s="66" t="str">
         <f>CONCATENATE(A131,A135,A139,A143)</f>
         <v/>
       </c>
@@ -59480,8 +59080,8 @@
         <v>262</v>
       </c>
       <c r="G131" s="18"/>
-      <c r="H131" s="67"/>
-      <c r="I131" s="64" t="str">
+      <c r="H131" s="64"/>
+      <c r="I131" s="66" t="str">
         <f>CONCATENATE(H131,H135,H139,H143)</f>
         <v/>
       </c>
@@ -59494,8 +59094,8 @@
         <v>262</v>
       </c>
       <c r="N131" s="18"/>
-      <c r="O131" s="67"/>
-      <c r="P131" s="64" t="str">
+      <c r="O131" s="64"/>
+      <c r="P131" s="66" t="str">
         <f>CONCATENATE(O131,O135,O139,O143)</f>
         <v/>
       </c>
@@ -59605,7 +59205,7 @@
       </c>
     </row>
     <row r="135" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="67"/>
+      <c r="A135" s="64"/>
       <c r="B135" s="65"/>
       <c r="C135" s="25"/>
       <c r="D135" s="35"/>
@@ -59615,7 +59215,7 @@
       <c r="F135" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="H135" s="67"/>
+      <c r="H135" s="64"/>
       <c r="I135" s="65"/>
       <c r="J135" s="36"/>
       <c r="K135" s="35"/>
@@ -59625,7 +59225,7 @@
       <c r="M135" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="O135" s="67"/>
+      <c r="O135" s="64"/>
       <c r="P135" s="65"/>
       <c r="Q135" s="25"/>
       <c r="R135" s="35"/>
@@ -59733,7 +59333,7 @@
       </c>
     </row>
     <row r="139" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A139" s="67"/>
+      <c r="A139" s="64"/>
       <c r="B139" s="65"/>
       <c r="C139" s="25"/>
       <c r="D139" s="35"/>
@@ -59743,7 +59343,7 @@
       <c r="F139" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="H139" s="67"/>
+      <c r="H139" s="64"/>
       <c r="I139" s="65"/>
       <c r="J139" s="36"/>
       <c r="K139" s="35"/>
@@ -59753,7 +59353,7 @@
       <c r="M139" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="O139" s="67"/>
+      <c r="O139" s="64"/>
       <c r="P139" s="65"/>
       <c r="Q139" s="25"/>
       <c r="R139" s="35"/>
@@ -59861,7 +59461,7 @@
       </c>
     </row>
     <row r="143" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="67"/>
+      <c r="A143" s="64"/>
       <c r="B143" s="65"/>
       <c r="C143" s="25"/>
       <c r="D143" s="35"/>
@@ -59871,7 +59471,7 @@
       <c r="F143" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="H143" s="67"/>
+      <c r="H143" s="64"/>
       <c r="I143" s="65"/>
       <c r="J143" s="36"/>
       <c r="K143" s="35"/>
@@ -59881,7 +59481,7 @@
       <c r="M143" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="O143" s="67"/>
+      <c r="O143" s="64"/>
       <c r="P143" s="65"/>
       <c r="Q143" s="25"/>
       <c r="R143" s="35"/>
@@ -59991,8 +59591,8 @@
       </c>
     </row>
     <row r="147" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A147" s="67"/>
-      <c r="B147" s="64" t="str">
+      <c r="A147" s="64"/>
+      <c r="B147" s="66" t="str">
         <f>CONCATENATE(A147,A151,A155,A159)</f>
         <v/>
       </c>
@@ -60005,8 +59605,8 @@
         <v>294</v>
       </c>
       <c r="G147" s="18"/>
-      <c r="H147" s="67"/>
-      <c r="I147" s="64" t="str">
+      <c r="H147" s="64"/>
+      <c r="I147" s="66" t="str">
         <f>CONCATENATE(H147,H151,H155,H159)</f>
         <v/>
       </c>
@@ -60019,8 +59619,8 @@
         <v>294</v>
       </c>
       <c r="N147" s="18"/>
-      <c r="O147" s="67"/>
-      <c r="P147" s="64" t="str">
+      <c r="O147" s="64"/>
+      <c r="P147" s="66" t="str">
         <f>CONCATENATE(O147,O151,O155,O159)</f>
         <v/>
       </c>
@@ -60130,7 +59730,7 @@
       </c>
     </row>
     <row r="151" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A151" s="67"/>
+      <c r="A151" s="64"/>
       <c r="B151" s="65"/>
       <c r="C151" s="25"/>
       <c r="D151" s="35"/>
@@ -60140,7 +59740,7 @@
       <c r="F151" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="H151" s="67"/>
+      <c r="H151" s="64"/>
       <c r="I151" s="65"/>
       <c r="J151" s="25"/>
       <c r="K151" s="35"/>
@@ -60150,7 +59750,7 @@
       <c r="M151" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="O151" s="67"/>
+      <c r="O151" s="64"/>
       <c r="P151" s="65"/>
       <c r="Q151" s="25"/>
       <c r="R151" s="35"/>
@@ -60258,7 +59858,7 @@
       </c>
     </row>
     <row r="155" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A155" s="67"/>
+      <c r="A155" s="64"/>
       <c r="B155" s="65"/>
       <c r="C155" s="25"/>
       <c r="D155" s="35"/>
@@ -60268,7 +59868,7 @@
       <c r="F155" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="H155" s="67"/>
+      <c r="H155" s="64"/>
       <c r="I155" s="65"/>
       <c r="J155" s="25"/>
       <c r="K155" s="35"/>
@@ -60278,7 +59878,7 @@
       <c r="M155" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="O155" s="67"/>
+      <c r="O155" s="64"/>
       <c r="P155" s="65"/>
       <c r="Q155" s="25"/>
       <c r="R155" s="35"/>
@@ -60386,7 +59986,7 @@
       </c>
     </row>
     <row r="159" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="67"/>
+      <c r="A159" s="64"/>
       <c r="B159" s="65"/>
       <c r="C159" s="25"/>
       <c r="D159" s="35"/>
@@ -60396,7 +59996,7 @@
       <c r="F159" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="H159" s="67"/>
+      <c r="H159" s="64"/>
       <c r="I159" s="65"/>
       <c r="J159" s="25"/>
       <c r="K159" s="35"/>
@@ -60406,7 +60006,7 @@
       <c r="M159" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="O159" s="67"/>
+      <c r="O159" s="64"/>
       <c r="P159" s="65"/>
       <c r="Q159" s="25"/>
       <c r="R159" s="35"/>
@@ -60516,8 +60116,8 @@
       </c>
     </row>
     <row r="163" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="67"/>
-      <c r="B163" s="64" t="str">
+      <c r="A163" s="64"/>
+      <c r="B163" s="66" t="str">
         <f>CONCATENATE(A163,A167,A171,A175)</f>
         <v/>
       </c>
@@ -60530,8 +60130,8 @@
         <v>326</v>
       </c>
       <c r="G163" s="18"/>
-      <c r="H163" s="67"/>
-      <c r="I163" s="64" t="str">
+      <c r="H163" s="64"/>
+      <c r="I163" s="66" t="str">
         <f>CONCATENATE(H163,H167,H171,H175)</f>
         <v/>
       </c>
@@ -60544,8 +60144,8 @@
         <v>326</v>
       </c>
       <c r="N163" s="18"/>
-      <c r="O163" s="67"/>
-      <c r="P163" s="64" t="str">
+      <c r="O163" s="64"/>
+      <c r="P163" s="66" t="str">
         <f>CONCATENATE(O163,O167,O171,O175)</f>
         <v/>
       </c>
@@ -60655,7 +60255,7 @@
       </c>
     </row>
     <row r="167" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A167" s="67"/>
+      <c r="A167" s="64"/>
       <c r="B167" s="65"/>
       <c r="C167" s="25"/>
       <c r="D167" s="35"/>
@@ -60665,7 +60265,7 @@
       <c r="F167" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="H167" s="67"/>
+      <c r="H167" s="64"/>
       <c r="I167" s="65"/>
       <c r="J167" s="25"/>
       <c r="K167" s="35"/>
@@ -60675,7 +60275,7 @@
       <c r="M167" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="O167" s="67"/>
+      <c r="O167" s="64"/>
       <c r="P167" s="65"/>
       <c r="Q167" s="25"/>
       <c r="R167" s="35"/>
@@ -60783,7 +60383,7 @@
       </c>
     </row>
     <row r="171" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="67"/>
+      <c r="A171" s="64"/>
       <c r="B171" s="65"/>
       <c r="C171" s="25"/>
       <c r="D171" s="35"/>
@@ -60793,7 +60393,7 @@
       <c r="F171" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="H171" s="67"/>
+      <c r="H171" s="64"/>
       <c r="I171" s="65"/>
       <c r="J171" s="25"/>
       <c r="K171" s="35"/>
@@ -60803,7 +60403,7 @@
       <c r="M171" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="O171" s="67"/>
+      <c r="O171" s="64"/>
       <c r="P171" s="65"/>
       <c r="Q171" s="25"/>
       <c r="R171" s="35"/>
@@ -60911,7 +60511,7 @@
       </c>
     </row>
     <row r="175" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A175" s="67"/>
+      <c r="A175" s="64"/>
       <c r="B175" s="65"/>
       <c r="C175" s="25"/>
       <c r="D175" s="35"/>
@@ -60921,7 +60521,7 @@
       <c r="F175" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="H175" s="67"/>
+      <c r="H175" s="64"/>
       <c r="I175" s="65"/>
       <c r="J175" s="25"/>
       <c r="K175" s="35"/>
@@ -60931,7 +60531,7 @@
       <c r="M175" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="O175" s="67"/>
+      <c r="O175" s="64"/>
       <c r="P175" s="65"/>
       <c r="Q175" s="25"/>
       <c r="R175" s="35"/>
@@ -61041,8 +60641,8 @@
       </c>
     </row>
     <row r="179" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A179" s="67"/>
-      <c r="B179" s="64" t="str">
+      <c r="A179" s="64"/>
+      <c r="B179" s="66" t="str">
         <f>CONCATENATE(A179,A183,A187,A191)</f>
         <v/>
       </c>
@@ -61055,8 +60655,8 @@
         <v>358</v>
       </c>
       <c r="G179" s="18"/>
-      <c r="H179" s="67"/>
-      <c r="I179" s="64" t="str">
+      <c r="H179" s="64"/>
+      <c r="I179" s="66" t="str">
         <f>CONCATENATE(H179,H183,H187,H191)</f>
         <v/>
       </c>
@@ -61069,8 +60669,8 @@
         <v>358</v>
       </c>
       <c r="N179" s="18"/>
-      <c r="O179" s="67"/>
-      <c r="P179" s="64" t="str">
+      <c r="O179" s="64"/>
+      <c r="P179" s="66" t="str">
         <f>CONCATENATE(O179,O183,O187,O191)</f>
         <v/>
       </c>
@@ -61180,7 +60780,7 @@
       </c>
     </row>
     <row r="183" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A183" s="67"/>
+      <c r="A183" s="64"/>
       <c r="B183" s="65"/>
       <c r="C183" s="25"/>
       <c r="D183" s="35"/>
@@ -61190,7 +60790,7 @@
       <c r="F183" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="H183" s="67"/>
+      <c r="H183" s="64"/>
       <c r="I183" s="65"/>
       <c r="J183" s="25"/>
       <c r="K183" s="35"/>
@@ -61200,7 +60800,7 @@
       <c r="M183" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="O183" s="67"/>
+      <c r="O183" s="64"/>
       <c r="P183" s="65"/>
       <c r="Q183" s="25"/>
       <c r="R183" s="35"/>
@@ -61308,7 +60908,7 @@
       </c>
     </row>
     <row r="187" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A187" s="67"/>
+      <c r="A187" s="64"/>
       <c r="B187" s="65"/>
       <c r="C187" s="25"/>
       <c r="D187" s="35"/>
@@ -61318,7 +60918,7 @@
       <c r="F187" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="H187" s="67"/>
+      <c r="H187" s="64"/>
       <c r="I187" s="65"/>
       <c r="J187" s="25"/>
       <c r="K187" s="35"/>
@@ -61328,7 +60928,7 @@
       <c r="M187" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="O187" s="67"/>
+      <c r="O187" s="64"/>
       <c r="P187" s="65"/>
       <c r="Q187" s="25"/>
       <c r="R187" s="35"/>
@@ -61436,7 +61036,7 @@
       </c>
     </row>
     <row r="191" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A191" s="67"/>
+      <c r="A191" s="64"/>
       <c r="B191" s="65"/>
       <c r="C191" s="25"/>
       <c r="D191" s="35"/>
@@ -61446,7 +61046,7 @@
       <c r="F191" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="H191" s="67"/>
+      <c r="H191" s="64"/>
       <c r="I191" s="65"/>
       <c r="J191" s="25"/>
       <c r="K191" s="35"/>
@@ -61456,7 +61056,7 @@
       <c r="M191" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="O191" s="67"/>
+      <c r="O191" s="64"/>
       <c r="P191" s="65"/>
       <c r="Q191" s="25"/>
       <c r="R191" s="35"/>
@@ -61566,8 +61166,8 @@
       </c>
     </row>
     <row r="195" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A195" s="67"/>
-      <c r="B195" s="64" t="str">
+      <c r="A195" s="64"/>
+      <c r="B195" s="66" t="str">
         <f>CONCATENATE(A195,A199,A203,A207)</f>
         <v/>
       </c>
@@ -61580,8 +61180,8 @@
         <v>390</v>
       </c>
       <c r="G195" s="18"/>
-      <c r="H195" s="67"/>
-      <c r="I195" s="64" t="str">
+      <c r="H195" s="64"/>
+      <c r="I195" s="66" t="str">
         <f>CONCATENATE(H195,H199,H203,H207)</f>
         <v/>
       </c>
@@ -61594,8 +61194,8 @@
         <v>390</v>
       </c>
       <c r="N195" s="18"/>
-      <c r="O195" s="67"/>
-      <c r="P195" s="64" t="str">
+      <c r="O195" s="64"/>
+      <c r="P195" s="66" t="str">
         <f>CONCATENATE(O195,O199,O203,O207)</f>
         <v/>
       </c>
@@ -61705,7 +61305,7 @@
       </c>
     </row>
     <row r="199" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A199" s="67"/>
+      <c r="A199" s="64"/>
       <c r="B199" s="65"/>
       <c r="C199" s="25"/>
       <c r="D199" s="5"/>
@@ -61715,7 +61315,7 @@
       <c r="F199" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="H199" s="67"/>
+      <c r="H199" s="64"/>
       <c r="I199" s="65"/>
       <c r="J199" s="25"/>
       <c r="K199" s="35"/>
@@ -61725,7 +61325,7 @@
       <c r="M199" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="O199" s="67"/>
+      <c r="O199" s="64"/>
       <c r="P199" s="65"/>
       <c r="Q199" s="25"/>
       <c r="R199" s="35"/>
@@ -61833,7 +61433,7 @@
       </c>
     </row>
     <row r="203" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A203" s="67"/>
+      <c r="A203" s="64"/>
       <c r="B203" s="65"/>
       <c r="C203" s="25"/>
       <c r="D203" s="5"/>
@@ -61843,7 +61443,7 @@
       <c r="F203" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="H203" s="67"/>
+      <c r="H203" s="64"/>
       <c r="I203" s="65"/>
       <c r="J203" s="25"/>
       <c r="K203" s="35"/>
@@ -61853,7 +61453,7 @@
       <c r="M203" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="O203" s="67"/>
+      <c r="O203" s="64"/>
       <c r="P203" s="65"/>
       <c r="Q203" s="25"/>
       <c r="R203" s="35"/>
@@ -61961,7 +61561,7 @@
       </c>
     </row>
     <row r="207" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A207" s="67"/>
+      <c r="A207" s="64"/>
       <c r="B207" s="65"/>
       <c r="C207" s="25"/>
       <c r="D207" s="5"/>
@@ -61971,7 +61571,7 @@
       <c r="F207" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="H207" s="67"/>
+      <c r="H207" s="64"/>
       <c r="I207" s="65"/>
       <c r="J207" s="25"/>
       <c r="K207" s="35"/>
@@ -61981,7 +61581,7 @@
       <c r="M207" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="O207" s="67"/>
+      <c r="O207" s="64"/>
       <c r="P207" s="65"/>
       <c r="Q207" s="25"/>
       <c r="R207" s="35"/>
@@ -62091,8 +61691,8 @@
       </c>
     </row>
     <row r="211" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A211" s="67"/>
-      <c r="B211" s="64" t="str">
+      <c r="A211" s="64"/>
+      <c r="B211" s="66" t="str">
         <f>CONCATENATE(A211,A215,A219,A223)</f>
         <v/>
       </c>
@@ -62105,8 +61705,8 @@
         <v>422</v>
       </c>
       <c r="G211" s="18"/>
-      <c r="H211" s="67"/>
-      <c r="I211" s="64" t="str">
+      <c r="H211" s="64"/>
+      <c r="I211" s="66" t="str">
         <f>CONCATENATE(H211,H215,H219,H223)</f>
         <v/>
       </c>
@@ -62119,8 +61719,8 @@
         <v>422</v>
       </c>
       <c r="N211" s="18"/>
-      <c r="O211" s="67"/>
-      <c r="P211" s="64" t="str">
+      <c r="O211" s="64"/>
+      <c r="P211" s="66" t="str">
         <f>CONCATENATE(O211,O215,O219,O223)</f>
         <v/>
       </c>
@@ -62230,7 +61830,7 @@
       </c>
     </row>
     <row r="215" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A215" s="67"/>
+      <c r="A215" s="64"/>
       <c r="B215" s="65"/>
       <c r="C215" s="25"/>
       <c r="D215" s="5"/>
@@ -62240,7 +61840,7 @@
       <c r="F215" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="H215" s="67"/>
+      <c r="H215" s="64"/>
       <c r="I215" s="65"/>
       <c r="J215" s="25"/>
       <c r="K215" s="35"/>
@@ -62250,7 +61850,7 @@
       <c r="M215" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="O215" s="67"/>
+      <c r="O215" s="64"/>
       <c r="P215" s="65"/>
       <c r="Q215" s="25"/>
       <c r="R215" s="35"/>
@@ -62358,7 +61958,7 @@
       </c>
     </row>
     <row r="219" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A219" s="67"/>
+      <c r="A219" s="64"/>
       <c r="B219" s="65"/>
       <c r="C219" s="25"/>
       <c r="D219" s="5"/>
@@ -62368,7 +61968,7 @@
       <c r="F219" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="H219" s="67"/>
+      <c r="H219" s="64"/>
       <c r="I219" s="65"/>
       <c r="J219" s="25"/>
       <c r="K219" s="35"/>
@@ -62378,7 +61978,7 @@
       <c r="M219" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="O219" s="67"/>
+      <c r="O219" s="64"/>
       <c r="P219" s="65"/>
       <c r="Q219" s="25"/>
       <c r="R219" s="35"/>
@@ -62486,7 +62086,7 @@
       </c>
     </row>
     <row r="223" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A223" s="67"/>
+      <c r="A223" s="64"/>
       <c r="B223" s="65"/>
       <c r="C223" s="25"/>
       <c r="D223" s="5"/>
@@ -62496,7 +62096,7 @@
       <c r="F223" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="H223" s="67"/>
+      <c r="H223" s="64"/>
       <c r="I223" s="65"/>
       <c r="J223" s="25"/>
       <c r="K223" s="35"/>
@@ -62506,7 +62106,7 @@
       <c r="M223" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="O223" s="67"/>
+      <c r="O223" s="64"/>
       <c r="P223" s="65"/>
       <c r="Q223" s="25"/>
       <c r="R223" s="35"/>
@@ -62616,8 +62216,8 @@
       </c>
     </row>
     <row r="227" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A227" s="67"/>
-      <c r="B227" s="64" t="str">
+      <c r="A227" s="64"/>
+      <c r="B227" s="66" t="str">
         <f>CONCATENATE(A227,A231,A235,A239)</f>
         <v/>
       </c>
@@ -62626,8 +62226,8 @@
       <c r="E227" s="17"/>
       <c r="F227" s="17"/>
       <c r="G227" s="18"/>
-      <c r="H227" s="67"/>
-      <c r="I227" s="64" t="str">
+      <c r="H227" s="64"/>
+      <c r="I227" s="66" t="str">
         <f>CONCATENATE(H227,H231,H235,H239)</f>
         <v/>
       </c>
@@ -62638,8 +62238,8 @@
         <v>454</v>
       </c>
       <c r="N227" s="18"/>
-      <c r="O227" s="67"/>
-      <c r="P227" s="64" t="str">
+      <c r="O227" s="64"/>
+      <c r="P227" s="66" t="str">
         <f>CONCATENATE(O227,O231,O235,O239)</f>
         <v/>
       </c>
@@ -62731,13 +62331,13 @@
       </c>
     </row>
     <row r="231" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A231" s="67"/>
+      <c r="A231" s="64"/>
       <c r="B231" s="65"/>
       <c r="C231" s="25"/>
       <c r="D231" s="5"/>
       <c r="E231" s="5"/>
       <c r="F231" s="5"/>
-      <c r="H231" s="67"/>
+      <c r="H231" s="64"/>
       <c r="I231" s="65"/>
       <c r="J231" s="1"/>
       <c r="K231" s="35"/>
@@ -62745,7 +62345,7 @@
       <c r="M231" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="O231" s="67"/>
+      <c r="O231" s="64"/>
       <c r="P231" s="65"/>
       <c r="Q231" s="25"/>
       <c r="R231" s="35"/>
@@ -62835,13 +62435,13 @@
       </c>
     </row>
     <row r="235" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A235" s="67"/>
+      <c r="A235" s="64"/>
       <c r="B235" s="65"/>
       <c r="C235" s="25"/>
       <c r="D235" s="5"/>
       <c r="E235" s="5"/>
       <c r="F235" s="5"/>
-      <c r="H235" s="67"/>
+      <c r="H235" s="64"/>
       <c r="I235" s="65"/>
       <c r="J235" s="1"/>
       <c r="K235" s="35"/>
@@ -62849,7 +62449,7 @@
       <c r="M235" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="O235" s="67"/>
+      <c r="O235" s="64"/>
       <c r="P235" s="65"/>
       <c r="Q235" s="25"/>
       <c r="R235" s="35"/>
@@ -62939,13 +62539,13 @@
       </c>
     </row>
     <row r="239" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A239" s="67"/>
+      <c r="A239" s="64"/>
       <c r="B239" s="65"/>
       <c r="C239" s="25"/>
       <c r="D239" s="5"/>
       <c r="E239" s="5"/>
       <c r="F239" s="5"/>
-      <c r="H239" s="67"/>
+      <c r="H239" s="64"/>
       <c r="I239" s="65"/>
       <c r="J239" s="1"/>
       <c r="K239" s="35"/>
@@ -62953,7 +62553,7 @@
       <c r="M239" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="O239" s="67"/>
+      <c r="O239" s="64"/>
       <c r="P239" s="65"/>
       <c r="Q239" s="25"/>
       <c r="R239" s="35"/>
@@ -63045,8 +62645,8 @@
       </c>
     </row>
     <row r="243" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A243" s="67"/>
-      <c r="B243" s="64" t="str">
+      <c r="A243" s="64"/>
+      <c r="B243" s="66" t="str">
         <f>CONCATENATE(A243,A247,A251,A255)</f>
         <v/>
       </c>
@@ -63055,8 +62655,8 @@
       <c r="E243" s="17"/>
       <c r="F243" s="17"/>
       <c r="G243" s="18"/>
-      <c r="H243" s="67"/>
-      <c r="I243" s="64" t="str">
+      <c r="H243" s="64"/>
+      <c r="I243" s="66" t="str">
         <f>CONCATENATE(H243,H247,H251,H255)</f>
         <v/>
       </c>
@@ -63067,8 +62667,8 @@
         <v>486</v>
       </c>
       <c r="N243" s="18"/>
-      <c r="O243" s="67"/>
-      <c r="P243" s="64" t="str">
+      <c r="O243" s="64"/>
+      <c r="P243" s="66" t="str">
         <f>CONCATENATE(O243,O247,O251,O255)</f>
         <v/>
       </c>
@@ -63160,13 +62760,13 @@
       </c>
     </row>
     <row r="247" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A247" s="67"/>
+      <c r="A247" s="64"/>
       <c r="B247" s="65"/>
       <c r="C247" s="25"/>
       <c r="D247" s="5"/>
       <c r="E247" s="5"/>
       <c r="F247" s="5"/>
-      <c r="H247" s="67"/>
+      <c r="H247" s="64"/>
       <c r="I247" s="65"/>
       <c r="J247" s="25"/>
       <c r="K247" s="35"/>
@@ -63174,7 +62774,7 @@
       <c r="M247" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="O247" s="67"/>
+      <c r="O247" s="64"/>
       <c r="P247" s="65"/>
       <c r="Q247" s="25"/>
       <c r="R247" s="35"/>
@@ -63264,13 +62864,13 @@
       </c>
     </row>
     <row r="251" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A251" s="67"/>
+      <c r="A251" s="64"/>
       <c r="B251" s="65"/>
       <c r="C251" s="25"/>
       <c r="D251" s="5"/>
       <c r="E251" s="5"/>
       <c r="F251" s="5"/>
-      <c r="H251" s="67"/>
+      <c r="H251" s="64"/>
       <c r="I251" s="65"/>
       <c r="J251" s="25"/>
       <c r="K251" s="35"/>
@@ -63278,7 +62878,7 @@
       <c r="M251" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="O251" s="67"/>
+      <c r="O251" s="64"/>
       <c r="P251" s="65"/>
       <c r="Q251" s="25"/>
       <c r="R251" s="35"/>
@@ -63368,13 +62968,13 @@
       </c>
     </row>
     <row r="255" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A255" s="67"/>
+      <c r="A255" s="64"/>
       <c r="B255" s="65"/>
       <c r="C255" s="25"/>
       <c r="D255" s="5"/>
       <c r="E255" s="5"/>
       <c r="F255" s="5"/>
-      <c r="H255" s="67"/>
+      <c r="H255" s="64"/>
       <c r="I255" s="65"/>
       <c r="J255" s="25"/>
       <c r="K255" s="35"/>
@@ -63382,7 +62982,7 @@
       <c r="M255" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="O255" s="67"/>
+      <c r="O255" s="64"/>
       <c r="P255" s="65"/>
       <c r="Q255" s="25"/>
       <c r="R255" s="35"/>
@@ -63474,8 +63074,8 @@
       </c>
     </row>
     <row r="259" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A259" s="67"/>
-      <c r="B259" s="64" t="str">
+      <c r="A259" s="64"/>
+      <c r="B259" s="66" t="str">
         <f>CONCATENATE(A259,A263,A267,A271)</f>
         <v/>
       </c>
@@ -63484,8 +63084,8 @@
       <c r="E259" s="17"/>
       <c r="F259" s="17"/>
       <c r="G259" s="18"/>
-      <c r="H259" s="67"/>
-      <c r="I259" s="64" t="str">
+      <c r="H259" s="64"/>
+      <c r="I259" s="66" t="str">
         <f>CONCATENATE(H259,H263,H267,H271)</f>
         <v/>
       </c>
@@ -63494,8 +63094,8 @@
       <c r="L259" s="17"/>
       <c r="M259" s="17"/>
       <c r="N259" s="18"/>
-      <c r="O259" s="67"/>
-      <c r="P259" s="64"/>
+      <c r="O259" s="64"/>
+      <c r="P259" s="66"/>
       <c r="Q259" s="25"/>
       <c r="R259" s="5"/>
       <c r="S259" s="17"/>
@@ -63562,19 +63162,19 @@
       <c r="T262" s="20"/>
     </row>
     <row r="263" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A263" s="67"/>
+      <c r="A263" s="64"/>
       <c r="B263" s="65"/>
       <c r="C263" s="25"/>
       <c r="D263" s="5"/>
       <c r="E263" s="5"/>
       <c r="F263" s="5"/>
-      <c r="H263" s="67"/>
+      <c r="H263" s="64"/>
       <c r="I263" s="65"/>
       <c r="J263" s="25"/>
       <c r="K263" s="5"/>
       <c r="L263" s="5"/>
       <c r="M263" s="5"/>
-      <c r="O263" s="67"/>
+      <c r="O263" s="64"/>
       <c r="P263" s="65"/>
       <c r="Q263" s="25"/>
       <c r="R263" s="5"/>
@@ -63642,19 +63242,19 @@
       <c r="T266" s="20"/>
     </row>
     <row r="267" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A267" s="67"/>
+      <c r="A267" s="64"/>
       <c r="B267" s="65"/>
       <c r="C267" s="25"/>
       <c r="D267" s="5"/>
       <c r="E267" s="5"/>
       <c r="F267" s="5"/>
-      <c r="H267" s="67"/>
+      <c r="H267" s="64"/>
       <c r="I267" s="65"/>
       <c r="J267" s="25"/>
       <c r="K267" s="5"/>
       <c r="L267" s="5"/>
       <c r="M267" s="5"/>
-      <c r="O267" s="67"/>
+      <c r="O267" s="64"/>
       <c r="P267" s="65"/>
       <c r="Q267" s="25"/>
       <c r="R267" s="5"/>
@@ -63722,19 +63322,19 @@
       <c r="T270" s="20"/>
     </row>
     <row r="271" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A271" s="67"/>
+      <c r="A271" s="64"/>
       <c r="B271" s="65"/>
       <c r="C271" s="25"/>
       <c r="D271" s="5"/>
       <c r="E271" s="5"/>
       <c r="F271" s="5"/>
-      <c r="H271" s="67"/>
+      <c r="H271" s="64"/>
       <c r="I271" s="65"/>
       <c r="J271" s="25"/>
       <c r="K271" s="5"/>
       <c r="L271" s="5"/>
       <c r="M271" s="5"/>
-      <c r="O271" s="67"/>
+      <c r="O271" s="64"/>
       <c r="P271" s="65"/>
       <c r="Q271" s="25"/>
       <c r="R271" s="5"/>
@@ -63804,8 +63404,8 @@
       <c r="T274" s="24"/>
     </row>
     <row r="275" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A275" s="67"/>
-      <c r="B275" s="64" t="str">
+      <c r="A275" s="64"/>
+      <c r="B275" s="66" t="str">
         <f>CONCATENATE(A275,A279,A283,A287)</f>
         <v/>
       </c>
@@ -63814,8 +63414,8 @@
       <c r="E275" s="17"/>
       <c r="F275" s="17"/>
       <c r="G275" s="18"/>
-      <c r="H275" s="67"/>
-      <c r="I275" s="64" t="str">
+      <c r="H275" s="64"/>
+      <c r="I275" s="66" t="str">
         <f>CONCATENATE(H275,H279,H283,H287)</f>
         <v/>
       </c>
@@ -63824,8 +63424,8 @@
       <c r="L275" s="17"/>
       <c r="M275" s="17"/>
       <c r="N275" s="18"/>
-      <c r="O275" s="67"/>
-      <c r="P275" s="64"/>
+      <c r="O275" s="64"/>
+      <c r="P275" s="66"/>
       <c r="Q275" s="25"/>
       <c r="R275" s="17"/>
       <c r="S275" s="17"/>
@@ -63892,19 +63492,19 @@
       <c r="T278" s="20"/>
     </row>
     <row r="279" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A279" s="67"/>
+      <c r="A279" s="64"/>
       <c r="B279" s="65"/>
       <c r="C279" s="25"/>
       <c r="D279" s="5"/>
       <c r="E279" s="5"/>
       <c r="F279" s="5"/>
-      <c r="H279" s="67"/>
+      <c r="H279" s="64"/>
       <c r="I279" s="65"/>
       <c r="J279" s="29"/>
       <c r="K279" s="5"/>
       <c r="L279" s="5"/>
       <c r="M279" s="5"/>
-      <c r="O279" s="67"/>
+      <c r="O279" s="64"/>
       <c r="P279" s="65"/>
       <c r="Q279" s="29"/>
       <c r="R279" s="5"/>
@@ -63972,19 +63572,19 @@
       <c r="T282" s="20"/>
     </row>
     <row r="283" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A283" s="67"/>
+      <c r="A283" s="64"/>
       <c r="B283" s="65"/>
       <c r="C283" s="1"/>
       <c r="D283" s="5"/>
       <c r="E283" s="5"/>
       <c r="F283" s="5"/>
-      <c r="H283" s="67"/>
+      <c r="H283" s="64"/>
       <c r="I283" s="65"/>
       <c r="J283" s="29"/>
       <c r="K283" s="5"/>
       <c r="L283" s="5"/>
       <c r="M283" s="5"/>
-      <c r="O283" s="67"/>
+      <c r="O283" s="64"/>
       <c r="P283" s="65"/>
       <c r="Q283" s="29"/>
       <c r="R283" s="5"/>
@@ -64052,19 +63652,19 @@
       <c r="T286" s="20"/>
     </row>
     <row r="287" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A287" s="67"/>
+      <c r="A287" s="64"/>
       <c r="B287" s="65"/>
       <c r="C287" s="1"/>
       <c r="D287" s="5"/>
       <c r="E287" s="5"/>
       <c r="F287" s="5"/>
-      <c r="H287" s="67"/>
+      <c r="H287" s="64"/>
       <c r="I287" s="65"/>
       <c r="J287" s="29"/>
       <c r="K287" s="5"/>
       <c r="L287" s="5"/>
       <c r="M287" s="5"/>
-      <c r="O287" s="67"/>
+      <c r="O287" s="64"/>
       <c r="P287" s="65"/>
       <c r="Q287" s="29"/>
       <c r="R287" s="5"/>
@@ -64134,8 +63734,8 @@
       <c r="T290" s="24"/>
     </row>
     <row r="291" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A291" s="67"/>
-      <c r="B291" s="64" t="str">
+      <c r="A291" s="64"/>
+      <c r="B291" s="66" t="str">
         <f>CONCATENATE(A291,A295,A299,A303)</f>
         <v/>
       </c>
@@ -64144,8 +63744,8 @@
       <c r="E291" s="17"/>
       <c r="F291" s="17"/>
       <c r="G291" s="18"/>
-      <c r="H291" s="67"/>
-      <c r="I291" s="64" t="str">
+      <c r="H291" s="64"/>
+      <c r="I291" s="66" t="str">
         <f>CONCATENATE(H291,H295,H299,H303)</f>
         <v/>
       </c>
@@ -64154,8 +63754,8 @@
       <c r="L291" s="17"/>
       <c r="M291" s="17"/>
       <c r="N291" s="18"/>
-      <c r="O291" s="67"/>
-      <c r="P291" s="64"/>
+      <c r="O291" s="64"/>
+      <c r="P291" s="66"/>
       <c r="Q291" s="28"/>
       <c r="R291" s="17"/>
       <c r="S291" s="17"/>
@@ -64222,19 +63822,19 @@
       <c r="T294" s="20"/>
     </row>
     <row r="295" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A295" s="67"/>
+      <c r="A295" s="64"/>
       <c r="B295" s="65"/>
       <c r="C295" s="1"/>
       <c r="D295" s="5"/>
       <c r="E295" s="5"/>
       <c r="F295" s="5"/>
-      <c r="H295" s="67"/>
+      <c r="H295" s="64"/>
       <c r="I295" s="65"/>
       <c r="J295" s="29"/>
       <c r="K295" s="5"/>
       <c r="L295" s="5"/>
       <c r="M295" s="5"/>
-      <c r="O295" s="67"/>
+      <c r="O295" s="64"/>
       <c r="P295" s="65"/>
       <c r="Q295" s="29"/>
       <c r="R295" s="5"/>
@@ -64302,19 +63902,19 @@
       <c r="T298" s="20"/>
     </row>
     <row r="299" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A299" s="67"/>
+      <c r="A299" s="64"/>
       <c r="B299" s="65"/>
       <c r="C299" s="1"/>
       <c r="D299" s="5"/>
       <c r="E299" s="5"/>
       <c r="F299" s="5"/>
-      <c r="H299" s="67"/>
+      <c r="H299" s="64"/>
       <c r="I299" s="65"/>
       <c r="J299" s="29"/>
       <c r="K299" s="5"/>
       <c r="L299" s="5"/>
       <c r="M299" s="5"/>
-      <c r="O299" s="67"/>
+      <c r="O299" s="64"/>
       <c r="P299" s="65"/>
       <c r="Q299" s="29"/>
       <c r="R299" s="5"/>
@@ -64382,19 +63982,19 @@
       <c r="T302" s="20"/>
     </row>
     <row r="303" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A303" s="67"/>
+      <c r="A303" s="64"/>
       <c r="B303" s="65"/>
       <c r="C303" s="1"/>
       <c r="D303" s="5"/>
       <c r="E303" s="5"/>
       <c r="F303" s="5"/>
-      <c r="H303" s="67"/>
+      <c r="H303" s="64"/>
       <c r="I303" s="65"/>
       <c r="J303" s="29"/>
       <c r="K303" s="5"/>
       <c r="L303" s="5"/>
       <c r="M303" s="5"/>
-      <c r="O303" s="67"/>
+      <c r="O303" s="64"/>
       <c r="P303" s="65"/>
       <c r="Q303" s="29"/>
       <c r="R303" s="5"/>
@@ -64464,8 +64064,8 @@
       <c r="T306" s="24"/>
     </row>
     <row r="307" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A307" s="72"/>
-      <c r="B307" s="64" t="str">
+      <c r="A307" s="67"/>
+      <c r="B307" s="66" t="str">
         <f>CONCATENATE(A307,A311,A315,A319)</f>
         <v/>
       </c>
@@ -64473,8 +64073,8 @@
       <c r="D307" s="12"/>
       <c r="E307" s="12"/>
       <c r="F307" s="12"/>
-      <c r="H307" s="72"/>
-      <c r="I307" s="64" t="str">
+      <c r="H307" s="67"/>
+      <c r="I307" s="66" t="str">
         <f>CONCATENATE(H307,H311,H315,H319)</f>
         <v/>
       </c>
@@ -64482,8 +64082,8 @@
       <c r="K307" s="12"/>
       <c r="L307" s="12"/>
       <c r="M307" s="12"/>
-      <c r="O307" s="72"/>
-      <c r="P307" s="66"/>
+      <c r="O307" s="67"/>
+      <c r="P307" s="72"/>
       <c r="Q307" s="31"/>
       <c r="R307" s="12"/>
       <c r="S307" s="12"/>
@@ -64552,11 +64152,11 @@
       <c r="T310" s="5"/>
     </row>
     <row r="311" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A311" s="67"/>
+      <c r="A311" s="64"/>
       <c r="B311" s="65"/>
-      <c r="H311" s="67"/>
+      <c r="H311" s="64"/>
       <c r="I311" s="65"/>
-      <c r="O311" s="67"/>
+      <c r="O311" s="64"/>
       <c r="P311" s="65"/>
     </row>
     <row r="312" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -64584,11 +64184,11 @@
       <c r="P314" s="65"/>
     </row>
     <row r="315" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A315" s="67"/>
+      <c r="A315" s="64"/>
       <c r="B315" s="65"/>
-      <c r="H315" s="67"/>
+      <c r="H315" s="64"/>
       <c r="I315" s="65"/>
-      <c r="O315" s="67"/>
+      <c r="O315" s="64"/>
       <c r="P315" s="65"/>
     </row>
     <row r="316" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -64616,11 +64216,11 @@
       <c r="P318" s="65"/>
     </row>
     <row r="319" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A319" s="67"/>
+      <c r="A319" s="64"/>
       <c r="B319" s="65"/>
-      <c r="H319" s="67"/>
+      <c r="H319" s="64"/>
       <c r="I319" s="65"/>
-      <c r="O319" s="67"/>
+      <c r="O319" s="64"/>
       <c r="P319" s="65"/>
     </row>
     <row r="320" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -64648,9 +64248,9 @@
       <c r="P322" s="61"/>
     </row>
     <row r="323" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B323" s="64"/>
-      <c r="I323" s="64"/>
-      <c r="P323" s="64"/>
+      <c r="B323" s="66"/>
+      <c r="I323" s="66"/>
+      <c r="P323" s="66"/>
     </row>
     <row r="324" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B324" s="65"/>
@@ -64729,6 +64329,288 @@
     </row>
   </sheetData>
   <mergeCells count="306">
+    <mergeCell ref="P227:P242"/>
+    <mergeCell ref="P243:P258"/>
+    <mergeCell ref="P259:P274"/>
+    <mergeCell ref="P275:P290"/>
+    <mergeCell ref="P291:P306"/>
+    <mergeCell ref="P307:P322"/>
+    <mergeCell ref="P131:P146"/>
+    <mergeCell ref="P147:P162"/>
+    <mergeCell ref="P163:P178"/>
+    <mergeCell ref="P179:P194"/>
+    <mergeCell ref="P195:P210"/>
+    <mergeCell ref="P211:P226"/>
+    <mergeCell ref="I323:I338"/>
+    <mergeCell ref="P3:P18"/>
+    <mergeCell ref="P19:P34"/>
+    <mergeCell ref="P35:P50"/>
+    <mergeCell ref="P51:P66"/>
+    <mergeCell ref="P67:P82"/>
+    <mergeCell ref="P83:P98"/>
+    <mergeCell ref="P99:P114"/>
+    <mergeCell ref="P115:P130"/>
+    <mergeCell ref="I211:I226"/>
+    <mergeCell ref="I227:I242"/>
+    <mergeCell ref="I243:I258"/>
+    <mergeCell ref="I259:I274"/>
+    <mergeCell ref="I275:I290"/>
+    <mergeCell ref="I291:I306"/>
+    <mergeCell ref="I115:I130"/>
+    <mergeCell ref="I131:I146"/>
+    <mergeCell ref="I147:I162"/>
+    <mergeCell ref="I163:I178"/>
+    <mergeCell ref="I179:I194"/>
+    <mergeCell ref="I195:I210"/>
+    <mergeCell ref="I3:I18"/>
+    <mergeCell ref="I19:I34"/>
+    <mergeCell ref="P323:P338"/>
+    <mergeCell ref="I51:I66"/>
+    <mergeCell ref="I67:I82"/>
+    <mergeCell ref="I83:I98"/>
+    <mergeCell ref="I99:I114"/>
+    <mergeCell ref="B291:B306"/>
+    <mergeCell ref="B307:B322"/>
+    <mergeCell ref="B323:B338"/>
+    <mergeCell ref="B195:B210"/>
+    <mergeCell ref="B211:B226"/>
+    <mergeCell ref="B227:B242"/>
+    <mergeCell ref="B243:B258"/>
+    <mergeCell ref="B259:B274"/>
+    <mergeCell ref="B275:B290"/>
+    <mergeCell ref="B99:B114"/>
+    <mergeCell ref="B115:B130"/>
+    <mergeCell ref="B131:B146"/>
+    <mergeCell ref="B147:B162"/>
+    <mergeCell ref="B163:B178"/>
+    <mergeCell ref="B179:B194"/>
+    <mergeCell ref="H311:H314"/>
+    <mergeCell ref="H315:H318"/>
+    <mergeCell ref="H319:H322"/>
+    <mergeCell ref="H239:H242"/>
+    <mergeCell ref="I307:I322"/>
+    <mergeCell ref="B19:B34"/>
+    <mergeCell ref="B35:B50"/>
+    <mergeCell ref="B51:B66"/>
+    <mergeCell ref="B67:B82"/>
+    <mergeCell ref="B83:B98"/>
+    <mergeCell ref="O319:O322"/>
+    <mergeCell ref="O1:T1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="O295:O298"/>
+    <mergeCell ref="O299:O302"/>
+    <mergeCell ref="O303:O306"/>
+    <mergeCell ref="O307:O310"/>
+    <mergeCell ref="O311:O314"/>
+    <mergeCell ref="O315:O318"/>
+    <mergeCell ref="O271:O274"/>
+    <mergeCell ref="O275:O278"/>
+    <mergeCell ref="O279:O282"/>
+    <mergeCell ref="O283:O286"/>
+    <mergeCell ref="O287:O290"/>
+    <mergeCell ref="O291:O294"/>
+    <mergeCell ref="O247:O250"/>
+    <mergeCell ref="O251:O254"/>
+    <mergeCell ref="I35:I50"/>
+    <mergeCell ref="O255:O258"/>
+    <mergeCell ref="O259:O262"/>
+    <mergeCell ref="O263:O266"/>
+    <mergeCell ref="O267:O270"/>
+    <mergeCell ref="O223:O226"/>
+    <mergeCell ref="O227:O230"/>
+    <mergeCell ref="O231:O234"/>
+    <mergeCell ref="O235:O238"/>
+    <mergeCell ref="O239:O242"/>
+    <mergeCell ref="O243:O246"/>
+    <mergeCell ref="O199:O202"/>
+    <mergeCell ref="O203:O206"/>
+    <mergeCell ref="O207:O210"/>
+    <mergeCell ref="O211:O214"/>
+    <mergeCell ref="O215:O218"/>
+    <mergeCell ref="O219:O222"/>
+    <mergeCell ref="O175:O178"/>
+    <mergeCell ref="O179:O182"/>
+    <mergeCell ref="O183:O186"/>
+    <mergeCell ref="O187:O190"/>
+    <mergeCell ref="O191:O194"/>
+    <mergeCell ref="O195:O198"/>
+    <mergeCell ref="O151:O154"/>
+    <mergeCell ref="O155:O158"/>
+    <mergeCell ref="O159:O162"/>
+    <mergeCell ref="O163:O166"/>
+    <mergeCell ref="O167:O170"/>
+    <mergeCell ref="O171:O174"/>
+    <mergeCell ref="O127:O130"/>
+    <mergeCell ref="O131:O134"/>
+    <mergeCell ref="O135:O138"/>
+    <mergeCell ref="O139:O142"/>
+    <mergeCell ref="O143:O146"/>
+    <mergeCell ref="O147:O150"/>
+    <mergeCell ref="O103:O106"/>
+    <mergeCell ref="O107:O110"/>
+    <mergeCell ref="O111:O114"/>
+    <mergeCell ref="O115:O118"/>
+    <mergeCell ref="O119:O122"/>
+    <mergeCell ref="O123:O126"/>
+    <mergeCell ref="O79:O82"/>
+    <mergeCell ref="O83:O86"/>
+    <mergeCell ref="O87:O90"/>
+    <mergeCell ref="O91:O94"/>
+    <mergeCell ref="O95:O98"/>
+    <mergeCell ref="O99:O102"/>
+    <mergeCell ref="O55:O58"/>
+    <mergeCell ref="O59:O62"/>
+    <mergeCell ref="O63:O66"/>
+    <mergeCell ref="O67:O70"/>
+    <mergeCell ref="O71:O74"/>
+    <mergeCell ref="O75:O78"/>
+    <mergeCell ref="O31:O34"/>
+    <mergeCell ref="O35:O38"/>
+    <mergeCell ref="O39:O42"/>
+    <mergeCell ref="O43:O46"/>
+    <mergeCell ref="O47:O50"/>
+    <mergeCell ref="O51:O54"/>
+    <mergeCell ref="H251:H254"/>
+    <mergeCell ref="H255:H258"/>
+    <mergeCell ref="H259:H262"/>
+    <mergeCell ref="H263:H266"/>
+    <mergeCell ref="H267:H270"/>
+    <mergeCell ref="H271:H274"/>
+    <mergeCell ref="H227:H230"/>
+    <mergeCell ref="H231:H234"/>
+    <mergeCell ref="H235:H238"/>
+    <mergeCell ref="H243:H246"/>
+    <mergeCell ref="H247:H250"/>
+    <mergeCell ref="H299:H302"/>
+    <mergeCell ref="H303:H306"/>
+    <mergeCell ref="H307:H310"/>
+    <mergeCell ref="H275:H278"/>
+    <mergeCell ref="H279:H282"/>
+    <mergeCell ref="H283:H286"/>
+    <mergeCell ref="H287:H290"/>
+    <mergeCell ref="H291:H294"/>
+    <mergeCell ref="H295:H298"/>
+    <mergeCell ref="H203:H206"/>
+    <mergeCell ref="H207:H210"/>
+    <mergeCell ref="H211:H214"/>
+    <mergeCell ref="H215:H218"/>
+    <mergeCell ref="H219:H222"/>
+    <mergeCell ref="H223:H226"/>
+    <mergeCell ref="H179:H182"/>
+    <mergeCell ref="H183:H186"/>
+    <mergeCell ref="H187:H190"/>
+    <mergeCell ref="H191:H194"/>
+    <mergeCell ref="H195:H198"/>
+    <mergeCell ref="H199:H202"/>
+    <mergeCell ref="H155:H158"/>
+    <mergeCell ref="H159:H162"/>
+    <mergeCell ref="H163:H166"/>
+    <mergeCell ref="H167:H170"/>
+    <mergeCell ref="H171:H174"/>
+    <mergeCell ref="H175:H178"/>
+    <mergeCell ref="H131:H134"/>
+    <mergeCell ref="H135:H138"/>
+    <mergeCell ref="H139:H142"/>
+    <mergeCell ref="H143:H146"/>
+    <mergeCell ref="H147:H150"/>
+    <mergeCell ref="H151:H154"/>
+    <mergeCell ref="H107:H110"/>
+    <mergeCell ref="H111:H114"/>
+    <mergeCell ref="H115:H118"/>
+    <mergeCell ref="H119:H122"/>
+    <mergeCell ref="H123:H126"/>
+    <mergeCell ref="H127:H130"/>
+    <mergeCell ref="H83:H86"/>
+    <mergeCell ref="H87:H90"/>
+    <mergeCell ref="H91:H94"/>
+    <mergeCell ref="H95:H98"/>
+    <mergeCell ref="H99:H102"/>
+    <mergeCell ref="H103:H106"/>
+    <mergeCell ref="H59:H62"/>
+    <mergeCell ref="H63:H66"/>
+    <mergeCell ref="H67:H70"/>
+    <mergeCell ref="H71:H74"/>
+    <mergeCell ref="H75:H78"/>
+    <mergeCell ref="H79:H82"/>
+    <mergeCell ref="H35:H38"/>
+    <mergeCell ref="H39:H42"/>
+    <mergeCell ref="H43:H46"/>
+    <mergeCell ref="H47:H50"/>
+    <mergeCell ref="H51:H54"/>
+    <mergeCell ref="H55:H58"/>
+    <mergeCell ref="A251:A254"/>
+    <mergeCell ref="A255:A258"/>
+    <mergeCell ref="A259:A262"/>
+    <mergeCell ref="A263:A266"/>
+    <mergeCell ref="A267:A270"/>
+    <mergeCell ref="A271:A274"/>
+    <mergeCell ref="A227:A230"/>
+    <mergeCell ref="A231:A234"/>
+    <mergeCell ref="A235:A238"/>
+    <mergeCell ref="A239:A242"/>
+    <mergeCell ref="A243:A246"/>
+    <mergeCell ref="A247:A250"/>
+    <mergeCell ref="A311:A314"/>
+    <mergeCell ref="A315:A318"/>
+    <mergeCell ref="A319:A322"/>
+    <mergeCell ref="A275:A278"/>
+    <mergeCell ref="A279:A282"/>
+    <mergeCell ref="A283:A286"/>
+    <mergeCell ref="A287:A290"/>
+    <mergeCell ref="A291:A294"/>
+    <mergeCell ref="A295:A298"/>
+    <mergeCell ref="A299:A302"/>
+    <mergeCell ref="A303:A306"/>
+    <mergeCell ref="A307:A310"/>
+    <mergeCell ref="A215:A218"/>
+    <mergeCell ref="A219:A222"/>
+    <mergeCell ref="A223:A226"/>
+    <mergeCell ref="A179:A182"/>
+    <mergeCell ref="A183:A186"/>
+    <mergeCell ref="A187:A190"/>
+    <mergeCell ref="A191:A194"/>
+    <mergeCell ref="A195:A198"/>
+    <mergeCell ref="A199:A202"/>
+    <mergeCell ref="A203:A206"/>
+    <mergeCell ref="A207:A210"/>
+    <mergeCell ref="A211:A214"/>
+    <mergeCell ref="A155:A158"/>
+    <mergeCell ref="A159:A162"/>
+    <mergeCell ref="A163:A166"/>
+    <mergeCell ref="A167:A170"/>
+    <mergeCell ref="A171:A174"/>
+    <mergeCell ref="A175:A178"/>
+    <mergeCell ref="A131:A134"/>
+    <mergeCell ref="A135:A138"/>
+    <mergeCell ref="A139:A142"/>
+    <mergeCell ref="A143:A146"/>
+    <mergeCell ref="A147:A150"/>
+    <mergeCell ref="A151:A154"/>
+    <mergeCell ref="A107:A110"/>
+    <mergeCell ref="A111:A114"/>
+    <mergeCell ref="A115:A118"/>
+    <mergeCell ref="A119:A122"/>
+    <mergeCell ref="A123:A126"/>
+    <mergeCell ref="A127:A130"/>
+    <mergeCell ref="A83:A86"/>
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="A91:A94"/>
+    <mergeCell ref="A95:A98"/>
+    <mergeCell ref="A99:A102"/>
+    <mergeCell ref="A103:A106"/>
+    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="A63:A66"/>
+    <mergeCell ref="A67:A70"/>
+    <mergeCell ref="A71:A74"/>
+    <mergeCell ref="A75:A78"/>
+    <mergeCell ref="A79:A82"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A55:A58"/>
     <mergeCell ref="O3:O6"/>
     <mergeCell ref="A11:A14"/>
     <mergeCell ref="A15:A18"/>
@@ -64753,288 +64635,6 @@
     <mergeCell ref="O23:O26"/>
     <mergeCell ref="O27:O30"/>
     <mergeCell ref="B3:B18"/>
-    <mergeCell ref="A59:A62"/>
-    <mergeCell ref="A63:A66"/>
-    <mergeCell ref="A67:A70"/>
-    <mergeCell ref="A71:A74"/>
-    <mergeCell ref="A75:A78"/>
-    <mergeCell ref="A79:A82"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="A55:A58"/>
-    <mergeCell ref="A107:A110"/>
-    <mergeCell ref="A111:A114"/>
-    <mergeCell ref="A115:A118"/>
-    <mergeCell ref="A119:A122"/>
-    <mergeCell ref="A123:A126"/>
-    <mergeCell ref="A127:A130"/>
-    <mergeCell ref="A83:A86"/>
-    <mergeCell ref="A87:A90"/>
-    <mergeCell ref="A91:A94"/>
-    <mergeCell ref="A95:A98"/>
-    <mergeCell ref="A99:A102"/>
-    <mergeCell ref="A103:A106"/>
-    <mergeCell ref="A155:A158"/>
-    <mergeCell ref="A159:A162"/>
-    <mergeCell ref="A163:A166"/>
-    <mergeCell ref="A167:A170"/>
-    <mergeCell ref="A171:A174"/>
-    <mergeCell ref="A175:A178"/>
-    <mergeCell ref="A131:A134"/>
-    <mergeCell ref="A135:A138"/>
-    <mergeCell ref="A139:A142"/>
-    <mergeCell ref="A143:A146"/>
-    <mergeCell ref="A147:A150"/>
-    <mergeCell ref="A151:A154"/>
-    <mergeCell ref="A215:A218"/>
-    <mergeCell ref="A219:A222"/>
-    <mergeCell ref="A223:A226"/>
-    <mergeCell ref="A179:A182"/>
-    <mergeCell ref="A183:A186"/>
-    <mergeCell ref="A187:A190"/>
-    <mergeCell ref="A191:A194"/>
-    <mergeCell ref="A195:A198"/>
-    <mergeCell ref="A199:A202"/>
-    <mergeCell ref="A203:A206"/>
-    <mergeCell ref="A207:A210"/>
-    <mergeCell ref="A211:A214"/>
-    <mergeCell ref="A311:A314"/>
-    <mergeCell ref="A315:A318"/>
-    <mergeCell ref="A319:A322"/>
-    <mergeCell ref="A275:A278"/>
-    <mergeCell ref="A279:A282"/>
-    <mergeCell ref="A283:A286"/>
-    <mergeCell ref="A287:A290"/>
-    <mergeCell ref="A291:A294"/>
-    <mergeCell ref="A295:A298"/>
-    <mergeCell ref="A299:A302"/>
-    <mergeCell ref="A303:A306"/>
-    <mergeCell ref="A307:A310"/>
-    <mergeCell ref="A251:A254"/>
-    <mergeCell ref="A255:A258"/>
-    <mergeCell ref="A259:A262"/>
-    <mergeCell ref="A263:A266"/>
-    <mergeCell ref="A267:A270"/>
-    <mergeCell ref="A271:A274"/>
-    <mergeCell ref="A227:A230"/>
-    <mergeCell ref="A231:A234"/>
-    <mergeCell ref="A235:A238"/>
-    <mergeCell ref="A239:A242"/>
-    <mergeCell ref="A243:A246"/>
-    <mergeCell ref="A247:A250"/>
-    <mergeCell ref="H59:H62"/>
-    <mergeCell ref="H63:H66"/>
-    <mergeCell ref="H67:H70"/>
-    <mergeCell ref="H71:H74"/>
-    <mergeCell ref="H75:H78"/>
-    <mergeCell ref="H79:H82"/>
-    <mergeCell ref="H35:H38"/>
-    <mergeCell ref="H39:H42"/>
-    <mergeCell ref="H43:H46"/>
-    <mergeCell ref="H47:H50"/>
-    <mergeCell ref="H51:H54"/>
-    <mergeCell ref="H55:H58"/>
-    <mergeCell ref="H107:H110"/>
-    <mergeCell ref="H111:H114"/>
-    <mergeCell ref="H115:H118"/>
-    <mergeCell ref="H119:H122"/>
-    <mergeCell ref="H123:H126"/>
-    <mergeCell ref="H127:H130"/>
-    <mergeCell ref="H83:H86"/>
-    <mergeCell ref="H87:H90"/>
-    <mergeCell ref="H91:H94"/>
-    <mergeCell ref="H95:H98"/>
-    <mergeCell ref="H99:H102"/>
-    <mergeCell ref="H103:H106"/>
-    <mergeCell ref="H155:H158"/>
-    <mergeCell ref="H159:H162"/>
-    <mergeCell ref="H163:H166"/>
-    <mergeCell ref="H167:H170"/>
-    <mergeCell ref="H171:H174"/>
-    <mergeCell ref="H175:H178"/>
-    <mergeCell ref="H131:H134"/>
-    <mergeCell ref="H135:H138"/>
-    <mergeCell ref="H139:H142"/>
-    <mergeCell ref="H143:H146"/>
-    <mergeCell ref="H147:H150"/>
-    <mergeCell ref="H151:H154"/>
-    <mergeCell ref="H203:H206"/>
-    <mergeCell ref="H207:H210"/>
-    <mergeCell ref="H211:H214"/>
-    <mergeCell ref="H215:H218"/>
-    <mergeCell ref="H219:H222"/>
-    <mergeCell ref="H223:H226"/>
-    <mergeCell ref="H179:H182"/>
-    <mergeCell ref="H183:H186"/>
-    <mergeCell ref="H187:H190"/>
-    <mergeCell ref="H191:H194"/>
-    <mergeCell ref="H195:H198"/>
-    <mergeCell ref="H199:H202"/>
-    <mergeCell ref="H299:H302"/>
-    <mergeCell ref="H303:H306"/>
-    <mergeCell ref="H307:H310"/>
-    <mergeCell ref="H275:H278"/>
-    <mergeCell ref="H279:H282"/>
-    <mergeCell ref="H283:H286"/>
-    <mergeCell ref="H287:H290"/>
-    <mergeCell ref="H291:H294"/>
-    <mergeCell ref="H295:H298"/>
-    <mergeCell ref="H251:H254"/>
-    <mergeCell ref="H255:H258"/>
-    <mergeCell ref="H259:H262"/>
-    <mergeCell ref="H263:H266"/>
-    <mergeCell ref="H267:H270"/>
-    <mergeCell ref="H271:H274"/>
-    <mergeCell ref="H227:H230"/>
-    <mergeCell ref="H231:H234"/>
-    <mergeCell ref="H235:H238"/>
-    <mergeCell ref="H243:H246"/>
-    <mergeCell ref="H247:H250"/>
-    <mergeCell ref="O55:O58"/>
-    <mergeCell ref="O59:O62"/>
-    <mergeCell ref="O63:O66"/>
-    <mergeCell ref="O67:O70"/>
-    <mergeCell ref="O71:O74"/>
-    <mergeCell ref="O75:O78"/>
-    <mergeCell ref="O31:O34"/>
-    <mergeCell ref="O35:O38"/>
-    <mergeCell ref="O39:O42"/>
-    <mergeCell ref="O43:O46"/>
-    <mergeCell ref="O47:O50"/>
-    <mergeCell ref="O51:O54"/>
-    <mergeCell ref="O103:O106"/>
-    <mergeCell ref="O107:O110"/>
-    <mergeCell ref="O111:O114"/>
-    <mergeCell ref="O115:O118"/>
-    <mergeCell ref="O119:O122"/>
-    <mergeCell ref="O123:O126"/>
-    <mergeCell ref="O79:O82"/>
-    <mergeCell ref="O83:O86"/>
-    <mergeCell ref="O87:O90"/>
-    <mergeCell ref="O91:O94"/>
-    <mergeCell ref="O95:O98"/>
-    <mergeCell ref="O99:O102"/>
-    <mergeCell ref="O151:O154"/>
-    <mergeCell ref="O155:O158"/>
-    <mergeCell ref="O159:O162"/>
-    <mergeCell ref="O163:O166"/>
-    <mergeCell ref="O167:O170"/>
-    <mergeCell ref="O171:O174"/>
-    <mergeCell ref="O127:O130"/>
-    <mergeCell ref="O131:O134"/>
-    <mergeCell ref="O135:O138"/>
-    <mergeCell ref="O139:O142"/>
-    <mergeCell ref="O143:O146"/>
-    <mergeCell ref="O147:O150"/>
-    <mergeCell ref="O199:O202"/>
-    <mergeCell ref="O203:O206"/>
-    <mergeCell ref="O207:O210"/>
-    <mergeCell ref="O211:O214"/>
-    <mergeCell ref="O215:O218"/>
-    <mergeCell ref="O219:O222"/>
-    <mergeCell ref="O175:O178"/>
-    <mergeCell ref="O179:O182"/>
-    <mergeCell ref="O183:O186"/>
-    <mergeCell ref="O187:O190"/>
-    <mergeCell ref="O191:O194"/>
-    <mergeCell ref="O195:O198"/>
-    <mergeCell ref="O255:O258"/>
-    <mergeCell ref="O259:O262"/>
-    <mergeCell ref="O263:O266"/>
-    <mergeCell ref="O267:O270"/>
-    <mergeCell ref="O223:O226"/>
-    <mergeCell ref="O227:O230"/>
-    <mergeCell ref="O231:O234"/>
-    <mergeCell ref="O235:O238"/>
-    <mergeCell ref="O239:O242"/>
-    <mergeCell ref="O243:O246"/>
-    <mergeCell ref="B19:B34"/>
-    <mergeCell ref="B35:B50"/>
-    <mergeCell ref="B51:B66"/>
-    <mergeCell ref="B67:B82"/>
-    <mergeCell ref="B83:B98"/>
-    <mergeCell ref="O319:O322"/>
-    <mergeCell ref="O1:T1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="O295:O298"/>
-    <mergeCell ref="O299:O302"/>
-    <mergeCell ref="O303:O306"/>
-    <mergeCell ref="O307:O310"/>
-    <mergeCell ref="O311:O314"/>
-    <mergeCell ref="O315:O318"/>
-    <mergeCell ref="O271:O274"/>
-    <mergeCell ref="O275:O278"/>
-    <mergeCell ref="O279:O282"/>
-    <mergeCell ref="O283:O286"/>
-    <mergeCell ref="O287:O290"/>
-    <mergeCell ref="O291:O294"/>
-    <mergeCell ref="O247:O250"/>
-    <mergeCell ref="O251:O254"/>
-    <mergeCell ref="I35:I50"/>
-    <mergeCell ref="I51:I66"/>
-    <mergeCell ref="I67:I82"/>
-    <mergeCell ref="I83:I98"/>
-    <mergeCell ref="I99:I114"/>
-    <mergeCell ref="B291:B306"/>
-    <mergeCell ref="B307:B322"/>
-    <mergeCell ref="B323:B338"/>
-    <mergeCell ref="B195:B210"/>
-    <mergeCell ref="B211:B226"/>
-    <mergeCell ref="B227:B242"/>
-    <mergeCell ref="B243:B258"/>
-    <mergeCell ref="B259:B274"/>
-    <mergeCell ref="B275:B290"/>
-    <mergeCell ref="B99:B114"/>
-    <mergeCell ref="B115:B130"/>
-    <mergeCell ref="B131:B146"/>
-    <mergeCell ref="B147:B162"/>
-    <mergeCell ref="B163:B178"/>
-    <mergeCell ref="B179:B194"/>
-    <mergeCell ref="H311:H314"/>
-    <mergeCell ref="H315:H318"/>
-    <mergeCell ref="H319:H322"/>
-    <mergeCell ref="H239:H242"/>
-    <mergeCell ref="I307:I322"/>
-    <mergeCell ref="I323:I338"/>
-    <mergeCell ref="P3:P18"/>
-    <mergeCell ref="P19:P34"/>
-    <mergeCell ref="P35:P50"/>
-    <mergeCell ref="P51:P66"/>
-    <mergeCell ref="P67:P82"/>
-    <mergeCell ref="P83:P98"/>
-    <mergeCell ref="P99:P114"/>
-    <mergeCell ref="P115:P130"/>
-    <mergeCell ref="I211:I226"/>
-    <mergeCell ref="I227:I242"/>
-    <mergeCell ref="I243:I258"/>
-    <mergeCell ref="I259:I274"/>
-    <mergeCell ref="I275:I290"/>
-    <mergeCell ref="I291:I306"/>
-    <mergeCell ref="I115:I130"/>
-    <mergeCell ref="I131:I146"/>
-    <mergeCell ref="I147:I162"/>
-    <mergeCell ref="I163:I178"/>
-    <mergeCell ref="I179:I194"/>
-    <mergeCell ref="I195:I210"/>
-    <mergeCell ref="I3:I18"/>
-    <mergeCell ref="I19:I34"/>
-    <mergeCell ref="P323:P338"/>
-    <mergeCell ref="P227:P242"/>
-    <mergeCell ref="P243:P258"/>
-    <mergeCell ref="P259:P274"/>
-    <mergeCell ref="P275:P290"/>
-    <mergeCell ref="P291:P306"/>
-    <mergeCell ref="P307:P322"/>
-    <mergeCell ref="P131:P146"/>
-    <mergeCell ref="P147:P162"/>
-    <mergeCell ref="P163:P178"/>
-    <mergeCell ref="P179:P194"/>
-    <mergeCell ref="P195:P210"/>
-    <mergeCell ref="P211:P226"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="17" scale="39" fitToHeight="0" orientation="portrait"/>

</xml_diff>